<commit_message>
Updated to put unused courses in approved electives
</commit_message>
<xml_diff>
--- a/blankPPF.xlsx
+++ b/blankPPF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshpopp/Downloads/ppfproj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2493D7F-D6E7-6E47-AE3B-03F68E88AD08}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB2D033-8F7D-374B-BDFD-5E55DBEA5F6E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1100" windowWidth="19500" windowHeight="14360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -639,7 +639,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -702,11 +702,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -749,49 +745,22 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -806,13 +775,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1153,8 +1148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49:I54"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M95" sqref="M95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -1175,54 +1170,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
       <c r="N1" s="20"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
       <c r="N2" s="2"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="67" t="s">
         <v>112</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="67"/>
-      <c r="M3" s="67"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
       <c r="N3" s="2"/>
     </row>
     <row r="5" spans="1:14">
@@ -1230,42 +1225,42 @@
         <v>11</v>
       </c>
       <c r="B5" s="66"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="67" t="s">
+      <c r="J5" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="67"/>
-      <c r="L5" s="77">
+      <c r="K5" s="63"/>
+      <c r="L5" s="68">
         <f ca="1">TODAY()</f>
-        <v>43671</v>
-      </c>
-      <c r="M5" s="77"/>
+        <v>43678</v>
+      </c>
+      <c r="M5" s="68"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="46" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="66"/>
       <c r="C6" s="66"/>
-      <c r="D6" s="80" t="s">
+      <c r="D6" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="81"/>
-      <c r="F6" s="81"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="82"/>
-      <c r="I6" s="82"/>
-      <c r="J6" s="67" t="s">
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="73"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="67"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="60"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="64"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="21" t="s">
@@ -1274,35 +1269,35 @@
       <c r="B7" s="66"/>
       <c r="C7" s="66"/>
       <c r="D7" s="66"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="67" t="s">
+      <c r="J7" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="K7" s="67"/>
-      <c r="L7" s="67"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="63"/>
       <c r="M7" s="24"/>
     </row>
     <row r="8" spans="1:14" ht="14" thickBot="1">
       <c r="A8" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="83"/>
-      <c r="C8" s="84"/>
-      <c r="D8" s="84"/>
-      <c r="J8" s="49" t="s">
+      <c r="B8" s="75"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="J8" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="K8" s="50"/>
+      <c r="K8" s="48"/>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="15"/>
-      <c r="B9" s="72" t="s">
+      <c r="B9" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="73"/>
+      <c r="C9" s="78"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -1320,10 +1315,10 @@
     </row>
     <row r="10" spans="1:14" ht="14" thickBot="1">
       <c r="A10" s="16"/>
-      <c r="B10" s="74" t="s">
+      <c r="B10" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="75"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -1347,12 +1342,12 @@
       <c r="A11" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="78" t="s">
+      <c r="B11" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="79"/>
-      <c r="E11" s="79"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
       <c r="F11" s="12"/>
     </row>
     <row r="12" spans="1:14">
@@ -1361,8 +1356,8 @@
         <v>16</v>
       </c>
       <c r="C12" s="66"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
       <c r="F12" s="2"/>
       <c r="G12" s="66" t="s">
         <v>99</v>
@@ -1377,8 +1372,8 @@
         <v>16</v>
       </c>
       <c r="C13" s="66"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
       <c r="F13" s="2"/>
       <c r="G13" s="66" t="s">
         <v>100</v>
@@ -1393,8 +1388,8 @@
         <v>38</v>
       </c>
       <c r="C14" s="66"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="60"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
       <c r="F14" s="2"/>
       <c r="G14" s="66" t="s">
         <v>52</v>
@@ -1409,8 +1404,8 @@
         <v>39</v>
       </c>
       <c r="C15" s="66"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
       <c r="F15" s="2"/>
       <c r="G15" s="66" t="s">
         <v>53</v>
@@ -1425,13 +1420,13 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="17"/>
-      <c r="B16" s="60" t="s">
+      <c r="B16" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="17"/>
@@ -1440,43 +1435,43 @@
       <c r="A18" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="67" t="s">
+      <c r="B18" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="17"/>
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
+      <c r="C19" s="64"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="64"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="60" t="s">
+      <c r="G19" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="H19" s="60"/>
+      <c r="H19" s="64"/>
       <c r="I19" s="6"/>
       <c r="K19" s="6"/>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="17"/>
-      <c r="B20" s="60" t="s">
+      <c r="B20" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="60" t="s">
+      <c r="G20" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="H20" s="60"/>
+      <c r="H20" s="64"/>
       <c r="I20" s="6"/>
       <c r="K20" s="7"/>
       <c r="M20" s="6">
@@ -1492,12 +1487,12 @@
       <c r="A22" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="67" t="s">
+      <c r="B22" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="60"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
       <c r="F22" s="2"/>
       <c r="I22" s="8"/>
       <c r="J22" s="13"/>
@@ -1507,30 +1502,30 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="17"/>
-      <c r="B23" s="60" t="s">
+      <c r="B23" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="61"/>
-      <c r="D23" s="61"/>
-      <c r="E23" s="61"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="60" t="s">
+      <c r="G23" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="H23" s="60"/>
+      <c r="H23" s="64"/>
       <c r="I23" s="6"/>
       <c r="K23" s="6"/>
       <c r="M23" s="8"/>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="17"/>
-      <c r="B24" s="60" t="s">
+      <c r="B24" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="61"/>
-      <c r="D24" s="61"/>
-      <c r="E24" s="61"/>
-      <c r="G24" s="41" t="s">
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="G24" s="39" t="s">
         <v>61</v>
       </c>
       <c r="I24" s="7"/>
@@ -1547,99 +1542,101 @@
       <c r="A26" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="67" t="s">
+      <c r="B26" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="60"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="60"/>
-      <c r="F26" s="60"/>
-      <c r="G26" s="60"/>
-      <c r="H26" s="60"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="56"/>
+      <c r="H26" s="56"/>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="17"/>
-      <c r="B27" s="60" t="s">
+      <c r="B27" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="60"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="60"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="60"/>
-      <c r="H27" s="60"/>
-      <c r="I27" s="6"/>
-      <c r="K27" s="6"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="59"/>
+      <c r="K27" s="59"/>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="17"/>
-      <c r="B28" s="60" t="s">
+      <c r="B28" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="60"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="60"/>
-      <c r="H28" s="60"/>
-      <c r="I28" s="7"/>
-      <c r="K28" s="7"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="55"/>
+      <c r="K28" s="55"/>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="17"/>
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="60"/>
-      <c r="H29" s="60"/>
-      <c r="I29" s="7"/>
-      <c r="K29" s="7"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="56"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="55"/>
+      <c r="K29" s="55"/>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="17"/>
       <c r="B30" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G30" s="60"/>
-      <c r="H30" s="60"/>
-      <c r="I30" s="7"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="55"/>
       <c r="J30" s="1"/>
-      <c r="K30" s="7"/>
+      <c r="K30" s="55"/>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="17"/>
-      <c r="B31" s="60" t="s">
+      <c r="B31" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="C31" s="60"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="60"/>
-      <c r="G31" s="60"/>
-      <c r="H31" s="60"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="8"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="56"/>
+      <c r="J31" s="56"/>
+      <c r="K31" s="56"/>
+      <c r="L31" s="56"/>
+      <c r="M31" s="56"/>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="17"/>
-      <c r="B32" s="62" t="s">
+      <c r="B32" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="60"/>
-      <c r="D32" s="60"/>
-      <c r="E32" s="60"/>
-      <c r="F32" s="61"/>
-      <c r="G32" s="60"/>
-      <c r="H32" s="60"/>
-      <c r="I32" s="6"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="56"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="59"/>
       <c r="J32" s="1"/>
-      <c r="K32" s="6"/>
-      <c r="M32" s="6">
+      <c r="K32" s="59"/>
+      <c r="M32" s="59">
         <f>SUM(K27:K32)</f>
         <v>0</v>
       </c>
@@ -1661,39 +1658,39 @@
       <c r="A34" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="42" t="s">
+      <c r="B34" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="41"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="39"/>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="17"/>
-      <c r="B35" s="60"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="60"/>
-      <c r="F35" s="61"/>
-      <c r="G35" s="60"/>
-      <c r="H35" s="60"/>
-      <c r="I35" s="6"/>
-      <c r="K35" s="6"/>
+      <c r="B35" s="56"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="56"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="56"/>
+      <c r="I35" s="59"/>
+      <c r="K35" s="59"/>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="17"/>
-      <c r="B36" s="60"/>
-      <c r="C36" s="60"/>
-      <c r="D36" s="60"/>
-      <c r="E36" s="60"/>
-      <c r="F36" s="61"/>
-      <c r="G36" s="60"/>
-      <c r="H36" s="60"/>
-      <c r="I36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="M36" s="6">
+      <c r="B36" s="56"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="56"/>
+      <c r="H36" s="56"/>
+      <c r="I36" s="55"/>
+      <c r="K36" s="55"/>
+      <c r="M36" s="59">
         <f>SUM(K35:K36)</f>
         <v>0</v>
       </c>
@@ -1715,20 +1712,20 @@
       <c r="A38" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="67" t="s">
+      <c r="B38" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="C38" s="60"/>
-      <c r="D38" s="60"/>
-      <c r="E38" s="60"/>
-      <c r="F38" s="60"/>
-      <c r="G38" s="60"/>
-      <c r="H38" s="60"/>
-      <c r="I38" s="61"/>
-      <c r="J38" s="61"/>
-      <c r="K38" s="61"/>
-      <c r="L38" s="61"/>
-      <c r="M38" s="61"/>
+      <c r="C38" s="64"/>
+      <c r="D38" s="64"/>
+      <c r="E38" s="64"/>
+      <c r="F38" s="64"/>
+      <c r="G38" s="64"/>
+      <c r="H38" s="64"/>
+      <c r="I38" s="65"/>
+      <c r="J38" s="65"/>
+      <c r="K38" s="65"/>
+      <c r="L38" s="65"/>
+      <c r="M38" s="65"/>
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="17"/>
@@ -1749,44 +1746,44 @@
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="17"/>
-      <c r="B40" s="34"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="34"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="35"/>
-      <c r="J40" s="35"/>
-      <c r="K40" s="35"/>
-      <c r="L40" s="35"/>
-      <c r="M40" s="35"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="34"/>
+      <c r="J40" s="34"/>
+      <c r="K40" s="34"/>
+      <c r="L40" s="34"/>
+      <c r="M40" s="34"/>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="17"/>
-      <c r="B41" s="63" t="s">
+      <c r="B41" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="C41" s="63"/>
-      <c r="D41" s="63"/>
-      <c r="E41" s="63"/>
-      <c r="F41" s="63"/>
-      <c r="G41" s="63"/>
-      <c r="H41" s="63"/>
+      <c r="C41" s="73"/>
+      <c r="D41" s="73"/>
+      <c r="E41" s="73"/>
+      <c r="F41" s="73"/>
+      <c r="G41" s="73"/>
+      <c r="H41" s="73"/>
       <c r="I41" s="8"/>
       <c r="K41" s="8"/>
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="17"/>
-      <c r="B42" s="63" t="s">
+      <c r="B42" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="63"/>
-      <c r="D42" s="63"/>
-      <c r="E42" s="63"/>
-      <c r="F42" s="63"/>
-      <c r="G42" s="63"/>
-      <c r="H42" s="63"/>
+      <c r="C42" s="73"/>
+      <c r="D42" s="73"/>
+      <c r="E42" s="73"/>
+      <c r="F42" s="73"/>
+      <c r="G42" s="73"/>
+      <c r="H42" s="73"/>
       <c r="I42" s="8"/>
       <c r="J42" s="13"/>
       <c r="K42" s="8"/>
@@ -1794,15 +1791,15 @@
     </row>
     <row r="43" spans="1:13">
       <c r="A43" s="17"/>
-      <c r="B43" s="63" t="s">
+      <c r="B43" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="63"/>
-      <c r="D43" s="63"/>
-      <c r="E43" s="63"/>
-      <c r="F43" s="63"/>
-      <c r="G43" s="63"/>
-      <c r="H43" s="63"/>
+      <c r="C43" s="73"/>
+      <c r="D43" s="73"/>
+      <c r="E43" s="73"/>
+      <c r="F43" s="73"/>
+      <c r="G43" s="73"/>
+      <c r="H43" s="73"/>
       <c r="I43" s="13"/>
       <c r="J43" s="13"/>
       <c r="K43" s="13"/>
@@ -1810,15 +1807,15 @@
     </row>
     <row r="44" spans="1:13">
       <c r="A44" s="17"/>
-      <c r="B44" s="63" t="s">
+      <c r="B44" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="C44" s="63"/>
-      <c r="D44" s="63"/>
-      <c r="E44" s="63"/>
-      <c r="F44" s="63"/>
-      <c r="G44" s="63"/>
-      <c r="H44" s="63"/>
+      <c r="C44" s="73"/>
+      <c r="D44" s="73"/>
+      <c r="E44" s="73"/>
+      <c r="F44" s="73"/>
+      <c r="G44" s="73"/>
+      <c r="H44" s="73"/>
       <c r="I44" s="13"/>
       <c r="J44" s="13"/>
       <c r="K44" s="13"/>
@@ -1826,15 +1823,15 @@
     </row>
     <row r="45" spans="1:13">
       <c r="A45" s="17"/>
-      <c r="B45" s="63" t="s">
+      <c r="B45" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="63"/>
-      <c r="D45" s="63"/>
-      <c r="E45" s="63"/>
-      <c r="F45" s="63"/>
-      <c r="G45" s="63"/>
-      <c r="H45" s="63"/>
+      <c r="C45" s="73"/>
+      <c r="D45" s="73"/>
+      <c r="E45" s="73"/>
+      <c r="F45" s="73"/>
+      <c r="G45" s="73"/>
+      <c r="H45" s="73"/>
       <c r="I45" s="8"/>
       <c r="J45" s="13"/>
       <c r="K45" s="8"/>
@@ -1842,15 +1839,15 @@
     </row>
     <row r="46" spans="1:13">
       <c r="A46" s="17"/>
-      <c r="B46" s="63" t="s">
+      <c r="B46" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="C46" s="63"/>
-      <c r="D46" s="63"/>
-      <c r="E46" s="63"/>
-      <c r="F46" s="63"/>
-      <c r="G46" s="63"/>
-      <c r="H46" s="63"/>
+      <c r="C46" s="73"/>
+      <c r="D46" s="73"/>
+      <c r="E46" s="73"/>
+      <c r="F46" s="73"/>
+      <c r="G46" s="73"/>
+      <c r="H46" s="73"/>
       <c r="I46" s="8"/>
       <c r="J46" s="13"/>
       <c r="K46" s="8"/>
@@ -1858,7 +1855,7 @@
     </row>
     <row r="47" spans="1:13">
       <c r="A47" s="17"/>
-      <c r="B47" s="37" t="s">
+      <c r="B47" s="35" t="s">
         <v>58</v>
       </c>
       <c r="I47" s="13"/>
@@ -1867,114 +1864,119 @@
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="17"/>
-      <c r="B48" s="60"/>
-      <c r="C48" s="60"/>
-      <c r="D48" s="60"/>
-      <c r="E48" s="60"/>
-      <c r="F48" s="34"/>
-      <c r="G48" s="60"/>
-      <c r="H48" s="60"/>
+      <c r="B48" s="64"/>
+      <c r="C48" s="64"/>
+      <c r="D48" s="64"/>
+      <c r="E48" s="64"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="64"/>
+      <c r="H48" s="64"/>
       <c r="I48" s="8"/>
       <c r="J48" s="13"/>
       <c r="K48" s="8"/>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="17"/>
-      <c r="B49" s="58"/>
-      <c r="C49" s="58"/>
-      <c r="D49" s="58"/>
-      <c r="E49" s="58"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="85"/>
-      <c r="H49" s="57"/>
-      <c r="I49" s="57"/>
-      <c r="K49" s="36"/>
+      <c r="B49" s="60"/>
+      <c r="C49" s="60"/>
+      <c r="D49" s="60"/>
+      <c r="E49" s="60"/>
+      <c r="F49" s="60"/>
+      <c r="G49" s="60"/>
+      <c r="H49" s="60"/>
+      <c r="I49" s="60"/>
+      <c r="J49" s="60"/>
+      <c r="K49" s="60"/>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="17"/>
-      <c r="B50" s="58"/>
-      <c r="C50" s="58"/>
-      <c r="D50" s="58"/>
-      <c r="E50" s="58"/>
-      <c r="F50" s="86"/>
-      <c r="G50" s="86"/>
-      <c r="H50" s="57"/>
-      <c r="I50" s="59"/>
-      <c r="K50" s="7"/>
+      <c r="B50" s="60"/>
+      <c r="C50" s="60"/>
+      <c r="D50" s="60"/>
+      <c r="E50" s="60"/>
+      <c r="F50" s="60"/>
+      <c r="G50" s="60"/>
+      <c r="H50" s="60"/>
+      <c r="I50" s="60"/>
+      <c r="J50" s="60"/>
+      <c r="K50" s="60"/>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="17"/>
-      <c r="B51" s="58"/>
-      <c r="C51" s="58"/>
-      <c r="D51" s="58"/>
-      <c r="E51" s="58"/>
-      <c r="F51" s="86"/>
-      <c r="G51" s="86"/>
-      <c r="H51" s="57"/>
-      <c r="I51" s="59"/>
-      <c r="K51" s="7"/>
+      <c r="B51" s="60"/>
+      <c r="C51" s="60"/>
+      <c r="D51" s="60"/>
+      <c r="E51" s="60"/>
+      <c r="F51" s="60"/>
+      <c r="G51" s="60"/>
+      <c r="H51" s="60"/>
+      <c r="I51" s="60"/>
+      <c r="J51" s="60"/>
+      <c r="K51" s="60"/>
     </row>
     <row r="52" spans="1:13">
       <c r="A52" s="17"/>
-      <c r="B52" s="58"/>
-      <c r="C52" s="58"/>
-      <c r="D52" s="58"/>
-      <c r="E52" s="58"/>
-      <c r="F52" s="86"/>
-      <c r="G52" s="86"/>
-      <c r="H52" s="57"/>
-      <c r="I52" s="57"/>
-      <c r="K52" s="36"/>
+      <c r="B52" s="60"/>
+      <c r="C52" s="60"/>
+      <c r="D52" s="60"/>
+      <c r="E52" s="60"/>
+      <c r="F52" s="60"/>
+      <c r="G52" s="60"/>
+      <c r="H52" s="60"/>
+      <c r="I52" s="60"/>
+      <c r="J52" s="60"/>
+      <c r="K52" s="60"/>
     </row>
     <row r="53" spans="1:13">
       <c r="A53" s="17"/>
-      <c r="B53" s="58"/>
-      <c r="C53" s="58"/>
-      <c r="D53" s="58"/>
-      <c r="E53" s="58"/>
-      <c r="F53" s="86"/>
-      <c r="G53" s="86"/>
-      <c r="H53" s="57"/>
-      <c r="I53" s="57"/>
-      <c r="J53" s="13"/>
-      <c r="K53" s="36"/>
+      <c r="B53" s="60"/>
+      <c r="C53" s="60"/>
+      <c r="D53" s="60"/>
+      <c r="E53" s="60"/>
+      <c r="F53" s="60"/>
+      <c r="G53" s="60"/>
+      <c r="H53" s="60"/>
+      <c r="I53" s="60"/>
+      <c r="J53" s="60"/>
+      <c r="K53" s="60"/>
       <c r="M53" s="8"/>
     </row>
     <row r="54" spans="1:13">
       <c r="A54" s="17"/>
-      <c r="B54" s="58"/>
-      <c r="C54" s="58"/>
-      <c r="D54" s="58"/>
-      <c r="E54" s="58"/>
-      <c r="F54" s="86"/>
-      <c r="G54" s="86"/>
-      <c r="H54" s="57"/>
-      <c r="I54" s="59"/>
-      <c r="K54" s="7"/>
+      <c r="B54" s="60"/>
+      <c r="C54" s="60"/>
+      <c r="D54" s="60"/>
+      <c r="E54" s="60"/>
+      <c r="F54" s="60"/>
+      <c r="G54" s="60"/>
+      <c r="H54" s="60"/>
+      <c r="I54" s="60"/>
+      <c r="J54" s="60"/>
+      <c r="K54" s="60"/>
       <c r="M54" s="8"/>
     </row>
     <row r="55" spans="1:13">
       <c r="A55" s="17"/>
-      <c r="B55" s="63"/>
-      <c r="C55" s="63"/>
-      <c r="D55" s="63"/>
-      <c r="E55" s="63"/>
-      <c r="F55" s="34"/>
-      <c r="G55" s="63"/>
-      <c r="H55" s="63"/>
+      <c r="B55" s="56"/>
+      <c r="C55" s="56"/>
+      <c r="D55" s="56"/>
+      <c r="E55" s="56"/>
+      <c r="F55" s="56"/>
+      <c r="G55" s="56"/>
+      <c r="H55" s="56"/>
       <c r="I55" s="8"/>
       <c r="K55" s="8"/>
       <c r="M55" s="8"/>
     </row>
     <row r="56" spans="1:13">
       <c r="A56" s="17"/>
-      <c r="B56" s="68"/>
-      <c r="C56" s="68"/>
-      <c r="D56" s="68"/>
-      <c r="E56" s="68"/>
-      <c r="F56" s="68"/>
-      <c r="G56" s="68"/>
-      <c r="H56" s="68"/>
+      <c r="B56" s="60"/>
+      <c r="C56" s="60"/>
+      <c r="D56" s="60"/>
+      <c r="E56" s="60"/>
+      <c r="F56" s="60"/>
+      <c r="G56" s="60"/>
+      <c r="H56" s="60"/>
       <c r="I56" s="8"/>
       <c r="J56" s="13"/>
       <c r="K56" s="8"/>
@@ -1990,9 +1992,9 @@
       <c r="F57" s="31"/>
       <c r="G57" s="31"/>
       <c r="H57" s="31"/>
-      <c r="I57" s="38"/>
-      <c r="J57" s="39"/>
-      <c r="K57" s="38"/>
+      <c r="I57" s="36"/>
+      <c r="J57" s="37"/>
+      <c r="K57" s="36"/>
       <c r="M57" s="6">
         <f>SUM(K41:K57)</f>
         <v>0</v>
@@ -2000,53 +2002,53 @@
     </row>
     <row r="58" spans="1:13">
       <c r="A58" s="17"/>
-      <c r="B58" s="54"/>
-      <c r="C58" s="54"/>
-      <c r="D58" s="54"/>
-      <c r="E58" s="54"/>
-      <c r="F58" s="54"/>
-      <c r="G58" s="54"/>
-      <c r="H58" s="54"/>
-      <c r="I58" s="38"/>
-      <c r="J58" s="39"/>
-      <c r="K58" s="38"/>
+      <c r="B58" s="52"/>
+      <c r="C58" s="52"/>
+      <c r="D58" s="52"/>
+      <c r="E58" s="52"/>
+      <c r="F58" s="52"/>
+      <c r="G58" s="52"/>
+      <c r="H58" s="52"/>
+      <c r="I58" s="36"/>
+      <c r="J58" s="37"/>
+      <c r="K58" s="36"/>
       <c r="M58" s="8"/>
     </row>
     <row r="59" spans="1:13">
       <c r="A59" s="17"/>
-      <c r="B59" s="54"/>
-      <c r="C59" s="54"/>
-      <c r="D59" s="54"/>
-      <c r="E59" s="54"/>
-      <c r="F59" s="54"/>
-      <c r="G59" s="54"/>
-      <c r="H59" s="54"/>
-      <c r="I59" s="38"/>
-      <c r="J59" s="39"/>
-      <c r="K59" s="38"/>
+      <c r="B59" s="52"/>
+      <c r="C59" s="52"/>
+      <c r="D59" s="52"/>
+      <c r="E59" s="52"/>
+      <c r="F59" s="52"/>
+      <c r="G59" s="52"/>
+      <c r="H59" s="52"/>
+      <c r="I59" s="36"/>
+      <c r="J59" s="37"/>
+      <c r="K59" s="36"/>
       <c r="M59" s="8"/>
     </row>
     <row r="60" spans="1:13">
       <c r="A60" s="17"/>
-      <c r="B60" s="63"/>
-      <c r="C60" s="63"/>
-      <c r="D60" s="63"/>
-      <c r="E60" s="63"/>
+      <c r="B60" s="73"/>
+      <c r="C60" s="73"/>
+      <c r="D60" s="73"/>
+      <c r="E60" s="73"/>
       <c r="F60" s="19"/>
-      <c r="G60" s="63"/>
-      <c r="H60" s="63"/>
+      <c r="G60" s="73"/>
+      <c r="H60" s="73"/>
       <c r="I60" s="8"/>
       <c r="K60" s="8"/>
     </row>
     <row r="61" spans="1:13">
       <c r="A61" s="17"/>
-      <c r="B61" s="40"/>
-      <c r="C61" s="40"/>
-      <c r="D61" s="40"/>
-      <c r="E61" s="40"/>
-      <c r="F61" s="40"/>
-      <c r="G61" s="40"/>
-      <c r="H61" s="40"/>
+      <c r="B61" s="38"/>
+      <c r="C61" s="38"/>
+      <c r="D61" s="38"/>
+      <c r="E61" s="38"/>
+      <c r="F61" s="38"/>
+      <c r="G61" s="38"/>
+      <c r="H61" s="38"/>
       <c r="I61" s="8"/>
       <c r="K61" s="8"/>
     </row>
@@ -2062,13 +2064,13 @@
       <c r="I62" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="J62" s="70">
+      <c r="J62" s="82">
         <f>B5</f>
         <v>0</v>
       </c>
-      <c r="K62" s="70"/>
-      <c r="L62" s="70"/>
-      <c r="M62" s="70"/>
+      <c r="K62" s="82"/>
+      <c r="L62" s="82"/>
+      <c r="M62" s="82"/>
     </row>
     <row r="63" spans="1:13">
       <c r="A63" s="17"/>
@@ -2089,27 +2091,27 @@
       <c r="A64" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B64" s="67" t="s">
+      <c r="B64" s="63" t="s">
         <v>105</v>
       </c>
-      <c r="C64" s="60"/>
-      <c r="D64" s="60"/>
-      <c r="E64" s="60"/>
+      <c r="C64" s="64"/>
+      <c r="D64" s="64"/>
+      <c r="E64" s="64"/>
       <c r="F64" s="2"/>
     </row>
     <row r="65" spans="1:13">
       <c r="A65" s="17"/>
-      <c r="B65" s="60" t="s">
+      <c r="B65" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="C65" s="60"/>
-      <c r="D65" s="60"/>
-      <c r="E65" s="60"/>
+      <c r="C65" s="64"/>
+      <c r="D65" s="64"/>
+      <c r="E65" s="64"/>
       <c r="F65" s="2"/>
-      <c r="G65" s="62" t="s">
+      <c r="G65" s="85" t="s">
         <v>98</v>
       </c>
-      <c r="H65" s="62"/>
+      <c r="H65" s="85"/>
       <c r="I65" s="6"/>
       <c r="K65" s="6"/>
       <c r="M65" s="6">
@@ -2124,10 +2126,10 @@
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
-      <c r="G66" s="62"/>
-      <c r="H66" s="61"/>
-      <c r="I66" s="52"/>
-      <c r="K66" s="52"/>
+      <c r="G66" s="85"/>
+      <c r="H66" s="65"/>
+      <c r="I66" s="50"/>
+      <c r="K66" s="50"/>
     </row>
     <row r="67" spans="1:13">
       <c r="A67" s="17"/>
@@ -2138,9 +2140,9 @@
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
-      <c r="I67" s="44"/>
-      <c r="J67" s="44"/>
-      <c r="K67" s="44"/>
+      <c r="I67" s="42"/>
+      <c r="J67" s="42"/>
+      <c r="K67" s="42"/>
       <c r="L67" s="18"/>
       <c r="M67" s="18"/>
     </row>
@@ -2148,216 +2150,216 @@
       <c r="A68" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B68" s="42" t="s">
+      <c r="B68" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="C68" s="41"/>
-      <c r="D68" s="41"/>
-      <c r="E68" s="41"/>
-      <c r="F68" s="41"/>
-      <c r="G68" s="41"/>
+      <c r="C68" s="39"/>
+      <c r="D68" s="39"/>
+      <c r="E68" s="39"/>
+      <c r="F68" s="39"/>
+      <c r="G68" s="39"/>
     </row>
     <row r="69" spans="1:13">
       <c r="A69" s="17"/>
-      <c r="B69" s="65" t="s">
+      <c r="B69" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="C69" s="65"/>
-      <c r="D69" s="65"/>
-      <c r="E69" s="65"/>
-      <c r="F69" s="65"/>
-      <c r="G69" s="65"/>
-      <c r="H69" s="65"/>
+      <c r="C69" s="84"/>
+      <c r="D69" s="84"/>
+      <c r="E69" s="84"/>
+      <c r="F69" s="84"/>
+      <c r="G69" s="84"/>
+      <c r="H69" s="84"/>
       <c r="I69" s="13"/>
       <c r="K69" s="13"/>
     </row>
     <row r="70" spans="1:13" ht="15">
       <c r="A70" s="17"/>
-      <c r="B70" s="60" t="s">
+      <c r="B70" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="C70" s="60"/>
-      <c r="D70" s="60"/>
-      <c r="E70" s="60"/>
+      <c r="C70" s="64"/>
+      <c r="D70" s="64"/>
+      <c r="E70" s="64"/>
       <c r="F70" s="2"/>
-      <c r="G70" s="60" t="s">
+      <c r="G70" s="64" t="s">
         <v>77</v>
       </c>
-      <c r="H70" s="60"/>
+      <c r="H70" s="64"/>
       <c r="I70" s="6"/>
       <c r="K70" s="6"/>
     </row>
     <row r="71" spans="1:13">
       <c r="A71" s="17"/>
-      <c r="B71" s="60" t="s">
+      <c r="B71" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="C71" s="60"/>
-      <c r="D71" s="60"/>
-      <c r="E71" s="60"/>
+      <c r="C71" s="64"/>
+      <c r="D71" s="64"/>
+      <c r="E71" s="64"/>
       <c r="F71" s="2"/>
-      <c r="G71" s="60" t="s">
+      <c r="G71" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="H71" s="60"/>
+      <c r="H71" s="64"/>
       <c r="I71" s="7"/>
       <c r="K71" s="7"/>
     </row>
     <row r="72" spans="1:13">
       <c r="A72" s="3"/>
-      <c r="B72" s="65" t="s">
+      <c r="B72" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="C72" s="65"/>
-      <c r="D72" s="65"/>
-      <c r="E72" s="65"/>
-      <c r="F72" s="65"/>
-      <c r="G72" s="65"/>
-      <c r="H72" s="65"/>
+      <c r="C72" s="84"/>
+      <c r="D72" s="84"/>
+      <c r="E72" s="84"/>
+      <c r="F72" s="84"/>
+      <c r="G72" s="84"/>
+      <c r="H72" s="84"/>
       <c r="I72" s="13"/>
       <c r="K72" s="13"/>
     </row>
     <row r="73" spans="1:13">
       <c r="A73" s="17"/>
-      <c r="B73" s="60" t="s">
+      <c r="B73" s="64" t="s">
         <v>107</v>
       </c>
-      <c r="C73" s="60"/>
-      <c r="D73" s="60"/>
-      <c r="E73" s="60"/>
+      <c r="C73" s="64"/>
+      <c r="D73" s="64"/>
+      <c r="E73" s="64"/>
       <c r="F73" s="2"/>
-      <c r="G73" s="60" t="s">
+      <c r="G73" s="64" t="s">
         <v>108</v>
       </c>
-      <c r="H73" s="60"/>
+      <c r="H73" s="64"/>
       <c r="I73" s="6"/>
       <c r="K73" s="6"/>
     </row>
     <row r="74" spans="1:13">
       <c r="A74" s="17"/>
-      <c r="B74" s="60" t="s">
+      <c r="B74" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="C74" s="60"/>
-      <c r="D74" s="60"/>
-      <c r="E74" s="60"/>
-      <c r="F74" s="45"/>
-      <c r="G74" s="60" t="s">
+      <c r="C74" s="64"/>
+      <c r="D74" s="64"/>
+      <c r="E74" s="64"/>
+      <c r="F74" s="43"/>
+      <c r="G74" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="H74" s="60"/>
-      <c r="I74" s="47"/>
-      <c r="K74" s="47"/>
+      <c r="H74" s="64"/>
+      <c r="I74" s="45"/>
+      <c r="K74" s="45"/>
     </row>
     <row r="75" spans="1:13">
       <c r="A75" s="17"/>
-      <c r="B75" s="45"/>
-      <c r="C75" s="45"/>
-      <c r="D75" s="45"/>
-      <c r="E75" s="45"/>
-      <c r="F75" s="45"/>
-      <c r="G75" s="45" t="s">
+      <c r="B75" s="43"/>
+      <c r="C75" s="43"/>
+      <c r="D75" s="43"/>
+      <c r="E75" s="43"/>
+      <c r="F75" s="43"/>
+      <c r="G75" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="H75" s="45"/>
-      <c r="I75" s="47"/>
-      <c r="K75" s="47"/>
+      <c r="H75" s="43"/>
+      <c r="I75" s="45"/>
+      <c r="K75" s="45"/>
     </row>
     <row r="76" spans="1:13" ht="13.5" customHeight="1">
       <c r="A76" s="17"/>
-      <c r="B76" s="63" t="s">
+      <c r="B76" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="C76" s="63"/>
-      <c r="D76" s="63"/>
-      <c r="E76" s="63"/>
-      <c r="F76" s="63"/>
-      <c r="G76" s="63" t="s">
+      <c r="C76" s="73"/>
+      <c r="D76" s="73"/>
+      <c r="E76" s="73"/>
+      <c r="F76" s="73"/>
+      <c r="G76" s="73" t="s">
         <v>79</v>
       </c>
-      <c r="H76" s="63"/>
+      <c r="H76" s="73"/>
       <c r="I76" s="7"/>
       <c r="J76" s="1"/>
       <c r="K76" s="7"/>
     </row>
     <row r="77" spans="1:13">
       <c r="A77" s="17"/>
-      <c r="B77" s="60" t="s">
+      <c r="B77" s="64" t="s">
         <v>96</v>
       </c>
-      <c r="C77" s="60"/>
-      <c r="D77" s="60"/>
-      <c r="E77" s="60"/>
-      <c r="F77" s="45"/>
-      <c r="G77" s="60" t="s">
+      <c r="C77" s="64"/>
+      <c r="D77" s="64"/>
+      <c r="E77" s="64"/>
+      <c r="F77" s="43"/>
+      <c r="G77" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="H77" s="60"/>
-      <c r="I77" s="47"/>
+      <c r="H77" s="64"/>
+      <c r="I77" s="45"/>
       <c r="J77" s="1"/>
-      <c r="K77" s="47"/>
+      <c r="K77" s="45"/>
     </row>
     <row r="78" spans="1:13">
       <c r="A78" s="17"/>
-      <c r="B78" s="46" t="s">
+      <c r="B78" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="D78" s="46"/>
-      <c r="E78" s="46"/>
-      <c r="F78" s="46"/>
-      <c r="G78" s="63" t="s">
+      <c r="D78" s="44"/>
+      <c r="E78" s="44"/>
+      <c r="F78" s="44"/>
+      <c r="G78" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="H78" s="63"/>
-      <c r="I78" s="47"/>
+      <c r="H78" s="73"/>
+      <c r="I78" s="45"/>
       <c r="J78" s="1"/>
-      <c r="K78" s="47"/>
+      <c r="K78" s="45"/>
     </row>
     <row r="79" spans="1:13">
       <c r="A79" s="17"/>
-      <c r="B79" s="60" t="s">
+      <c r="B79" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="C79" s="60"/>
-      <c r="D79" s="60"/>
-      <c r="E79" s="60"/>
+      <c r="C79" s="64"/>
+      <c r="D79" s="64"/>
+      <c r="E79" s="64"/>
       <c r="F79" s="2"/>
-      <c r="G79" s="60" t="s">
+      <c r="G79" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="H79" s="60"/>
+      <c r="H79" s="64"/>
       <c r="I79" s="6"/>
       <c r="K79" s="6"/>
     </row>
     <row r="80" spans="1:13">
       <c r="A80" s="17"/>
-      <c r="B80" s="60" t="s">
+      <c r="B80" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="C80" s="60"/>
-      <c r="D80" s="60"/>
-      <c r="E80" s="60"/>
+      <c r="C80" s="64"/>
+      <c r="D80" s="64"/>
+      <c r="E80" s="64"/>
       <c r="F80" s="2"/>
-      <c r="G80" s="60" t="s">
+      <c r="G80" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="H80" s="60"/>
+      <c r="H80" s="64"/>
       <c r="I80" s="8"/>
       <c r="K80" s="8"/>
     </row>
     <row r="81" spans="1:13">
       <c r="A81" s="17"/>
-      <c r="B81" s="60" t="s">
+      <c r="B81" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="C81" s="60"/>
-      <c r="D81" s="60"/>
-      <c r="E81" s="60"/>
+      <c r="C81" s="64"/>
+      <c r="D81" s="64"/>
+      <c r="E81" s="64"/>
       <c r="F81" s="2"/>
-      <c r="G81" s="60" t="s">
+      <c r="G81" s="64" t="s">
         <v>85</v>
       </c>
-      <c r="H81" s="60"/>
+      <c r="H81" s="64"/>
       <c r="I81" s="7"/>
       <c r="K81" s="7"/>
     </row>
@@ -2374,111 +2376,111 @@
     </row>
     <row r="83" spans="1:13">
       <c r="A83" s="17"/>
-      <c r="B83" s="60" t="s">
+      <c r="B83" s="64" t="s">
         <v>111</v>
       </c>
-      <c r="C83" s="60"/>
-      <c r="D83" s="60"/>
-      <c r="E83" s="60"/>
-      <c r="F83" s="60"/>
-      <c r="G83" s="60"/>
-      <c r="H83" s="60"/>
-      <c r="I83" s="61"/>
-      <c r="J83" s="61"/>
-      <c r="K83" s="61"/>
+      <c r="C83" s="64"/>
+      <c r="D83" s="64"/>
+      <c r="E83" s="64"/>
+      <c r="F83" s="64"/>
+      <c r="G83" s="64"/>
+      <c r="H83" s="64"/>
+      <c r="I83" s="65"/>
+      <c r="J83" s="65"/>
+      <c r="K83" s="65"/>
     </row>
     <row r="84" spans="1:13">
       <c r="A84" s="17"/>
-      <c r="B84" s="60" t="s">
+      <c r="B84" s="64" t="s">
         <v>89</v>
       </c>
-      <c r="C84" s="60"/>
-      <c r="D84" s="60"/>
-      <c r="E84" s="60"/>
+      <c r="C84" s="64"/>
+      <c r="D84" s="64"/>
+      <c r="E84" s="64"/>
       <c r="F84" s="2"/>
-      <c r="G84" s="60"/>
-      <c r="H84" s="60"/>
+      <c r="G84" s="56"/>
+      <c r="H84" s="56"/>
       <c r="I84" s="6"/>
       <c r="J84" s="1"/>
       <c r="K84" s="6"/>
     </row>
     <row r="85" spans="1:13">
       <c r="A85" s="17"/>
-      <c r="B85" s="60" t="s">
+      <c r="B85" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="C85" s="60"/>
-      <c r="D85" s="60"/>
-      <c r="E85" s="60"/>
+      <c r="C85" s="64"/>
+      <c r="D85" s="64"/>
+      <c r="E85" s="64"/>
       <c r="F85" s="2"/>
-      <c r="G85" s="60"/>
-      <c r="H85" s="60"/>
+      <c r="G85" s="56"/>
+      <c r="H85" s="56"/>
       <c r="I85" s="6"/>
       <c r="K85" s="6"/>
     </row>
     <row r="86" spans="1:13">
       <c r="A86" s="17"/>
-      <c r="B86" s="60" t="s">
+      <c r="B86" s="64" t="s">
         <v>91</v>
       </c>
-      <c r="C86" s="60"/>
-      <c r="D86" s="60"/>
-      <c r="E86" s="60"/>
+      <c r="C86" s="64"/>
+      <c r="D86" s="64"/>
+      <c r="E86" s="64"/>
       <c r="F86" s="2"/>
-      <c r="G86" s="60"/>
-      <c r="H86" s="60"/>
+      <c r="G86" s="56"/>
+      <c r="H86" s="56"/>
       <c r="I86" s="6"/>
       <c r="K86" s="6"/>
     </row>
     <row r="87" spans="1:13">
       <c r="A87" s="17"/>
-      <c r="B87" s="60" t="s">
+      <c r="B87" s="64" t="s">
         <v>92</v>
       </c>
-      <c r="C87" s="60"/>
-      <c r="D87" s="60"/>
-      <c r="E87" s="60"/>
-      <c r="F87" s="45"/>
-      <c r="G87" s="45"/>
-      <c r="H87" s="45"/>
-      <c r="I87" s="53"/>
-      <c r="K87" s="53"/>
+      <c r="C87" s="64"/>
+      <c r="D87" s="64"/>
+      <c r="E87" s="64"/>
+      <c r="F87" s="43"/>
+      <c r="G87" s="43"/>
+      <c r="H87" s="43"/>
+      <c r="I87" s="51"/>
+      <c r="K87" s="51"/>
     </row>
     <row r="88" spans="1:13">
       <c r="A88" s="17"/>
-      <c r="B88" s="60" t="s">
+      <c r="B88" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="C88" s="60"/>
-      <c r="D88" s="60"/>
-      <c r="E88" s="60"/>
-      <c r="F88" s="45"/>
-      <c r="G88" s="45"/>
-      <c r="H88" s="45"/>
+      <c r="C88" s="64"/>
+      <c r="D88" s="64"/>
+      <c r="E88" s="64"/>
+      <c r="F88" s="43"/>
+      <c r="G88" s="43"/>
+      <c r="H88" s="43"/>
       <c r="I88" s="8"/>
       <c r="K88" s="8"/>
     </row>
     <row r="89" spans="1:13">
       <c r="A89" s="17"/>
-      <c r="B89" s="60"/>
-      <c r="C89" s="60"/>
-      <c r="D89" s="60"/>
-      <c r="E89" s="60"/>
-      <c r="F89" s="61"/>
-      <c r="G89" s="60"/>
-      <c r="H89" s="60"/>
+      <c r="B89" s="64"/>
+      <c r="C89" s="64"/>
+      <c r="D89" s="64"/>
+      <c r="E89" s="64"/>
+      <c r="F89" s="65"/>
+      <c r="G89" s="64"/>
+      <c r="H89" s="64"/>
       <c r="I89" s="7"/>
       <c r="K89" s="7"/>
     </row>
     <row r="90" spans="1:13">
       <c r="A90" s="17"/>
-      <c r="B90" s="60"/>
-      <c r="C90" s="60"/>
-      <c r="D90" s="60"/>
-      <c r="E90" s="60"/>
-      <c r="F90" s="61"/>
-      <c r="G90" s="60"/>
-      <c r="H90" s="60"/>
+      <c r="B90" s="64"/>
+      <c r="C90" s="64"/>
+      <c r="D90" s="64"/>
+      <c r="E90" s="64"/>
+      <c r="F90" s="65"/>
+      <c r="G90" s="64"/>
+      <c r="H90" s="64"/>
       <c r="I90" s="7"/>
       <c r="K90" s="7"/>
       <c r="M90" s="6">
@@ -2493,47 +2495,47 @@
       <c r="A92" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B92" s="67" t="s">
+      <c r="B92" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="C92" s="60"/>
-      <c r="D92" s="60"/>
-      <c r="E92" s="60"/>
+      <c r="C92" s="64"/>
+      <c r="D92" s="64"/>
+      <c r="E92" s="64"/>
       <c r="F92" s="2"/>
     </row>
     <row r="93" spans="1:13">
       <c r="A93" s="17"/>
-      <c r="B93" s="60"/>
-      <c r="C93" s="60"/>
-      <c r="D93" s="60"/>
-      <c r="E93" s="60"/>
-      <c r="F93" s="61"/>
-      <c r="G93" s="71"/>
-      <c r="H93" s="71"/>
+      <c r="B93" s="56"/>
+      <c r="C93" s="56"/>
+      <c r="D93" s="56"/>
+      <c r="E93" s="56"/>
+      <c r="F93" s="57"/>
+      <c r="G93" s="62"/>
+      <c r="H93" s="62"/>
       <c r="I93" s="32"/>
       <c r="K93" s="6"/>
     </row>
     <row r="94" spans="1:13">
       <c r="A94" s="17"/>
-      <c r="B94" s="60"/>
-      <c r="C94" s="60"/>
-      <c r="D94" s="60"/>
-      <c r="E94" s="60"/>
-      <c r="F94" s="61"/>
-      <c r="G94" s="60"/>
-      <c r="H94" s="60"/>
+      <c r="B94" s="56"/>
+      <c r="C94" s="56"/>
+      <c r="D94" s="56"/>
+      <c r="E94" s="56"/>
+      <c r="F94" s="57"/>
+      <c r="G94" s="56"/>
+      <c r="H94" s="56"/>
       <c r="I94" s="6"/>
       <c r="K94" s="6"/>
     </row>
     <row r="95" spans="1:13">
       <c r="A95" s="17"/>
-      <c r="B95" s="60"/>
-      <c r="C95" s="60"/>
-      <c r="D95" s="60"/>
-      <c r="E95" s="60"/>
-      <c r="F95" s="61"/>
-      <c r="G95" s="60"/>
-      <c r="H95" s="60"/>
+      <c r="B95" s="56"/>
+      <c r="C95" s="56"/>
+      <c r="D95" s="56"/>
+      <c r="E95" s="56"/>
+      <c r="F95" s="57"/>
+      <c r="G95" s="56"/>
+      <c r="H95" s="56"/>
       <c r="I95" s="7"/>
       <c r="K95" s="7"/>
       <c r="M95" s="6">
@@ -2556,21 +2558,21 @@
     </row>
     <row r="97" spans="1:13">
       <c r="A97" s="17"/>
-      <c r="B97" s="60"/>
-      <c r="C97" s="60"/>
-      <c r="D97" s="60"/>
-      <c r="E97" s="60"/>
-      <c r="F97" s="60"/>
-      <c r="G97" s="60"/>
-      <c r="H97" s="60"/>
-      <c r="I97" s="60"/>
-      <c r="J97" s="60"/>
-      <c r="K97" s="60"/>
+      <c r="B97" s="64"/>
+      <c r="C97" s="64"/>
+      <c r="D97" s="64"/>
+      <c r="E97" s="64"/>
+      <c r="F97" s="64"/>
+      <c r="G97" s="64"/>
+      <c r="H97" s="64"/>
+      <c r="I97" s="64"/>
+      <c r="J97" s="64"/>
+      <c r="K97" s="64"/>
     </row>
     <row r="98" spans="1:13">
       <c r="A98" s="17"/>
       <c r="I98" s="1"/>
-      <c r="J98" s="43" t="s">
+      <c r="J98" s="41" t="s">
         <v>9</v>
       </c>
       <c r="K98" s="1"/>
@@ -2584,49 +2586,49 @@
       <c r="A99" s="17"/>
       <c r="J99" s="23"/>
       <c r="K99" s="25"/>
-      <c r="L99" s="69" t="s">
+      <c r="L99" s="81" t="s">
         <v>110</v>
       </c>
-      <c r="M99" s="69"/>
+      <c r="M99" s="81"/>
     </row>
     <row r="100" spans="1:13">
       <c r="A100" s="17"/>
       <c r="B100" s="6"/>
-      <c r="C100" s="60" t="s">
+      <c r="C100" s="64" t="s">
         <v>73</v>
       </c>
-      <c r="D100" s="60"/>
-      <c r="E100" s="61"/>
-      <c r="F100" s="61"/>
-      <c r="G100" s="61"/>
-      <c r="H100" s="64"/>
-      <c r="I100" s="64"/>
+      <c r="D100" s="64"/>
+      <c r="E100" s="65"/>
+      <c r="F100" s="65"/>
+      <c r="G100" s="65"/>
+      <c r="H100" s="83"/>
+      <c r="I100" s="83"/>
     </row>
     <row r="101" spans="1:13">
       <c r="A101" s="17"/>
       <c r="B101" s="7"/>
-      <c r="C101" s="60" t="s">
+      <c r="C101" s="64" t="s">
         <v>74</v>
       </c>
-      <c r="D101" s="60"/>
-      <c r="E101" s="60"/>
-      <c r="F101" s="60"/>
-      <c r="G101" s="60"/>
-      <c r="H101" s="64"/>
-      <c r="I101" s="64"/>
+      <c r="D101" s="64"/>
+      <c r="E101" s="64"/>
+      <c r="F101" s="64"/>
+      <c r="G101" s="64"/>
+      <c r="H101" s="83"/>
+      <c r="I101" s="83"/>
     </row>
     <row r="102" spans="1:13">
       <c r="A102" s="17"/>
       <c r="B102" s="7"/>
-      <c r="C102" s="60" t="s">
+      <c r="C102" s="64" t="s">
         <v>75</v>
       </c>
-      <c r="D102" s="61"/>
-      <c r="E102" s="61"/>
-      <c r="F102" s="61"/>
-      <c r="G102" s="61"/>
-      <c r="H102" s="64"/>
-      <c r="I102" s="64"/>
+      <c r="D102" s="65"/>
+      <c r="E102" s="65"/>
+      <c r="F102" s="65"/>
+      <c r="G102" s="65"/>
+      <c r="H102" s="83"/>
+      <c r="I102" s="83"/>
     </row>
     <row r="103" spans="1:13">
       <c r="A103" s="17"/>
@@ -2640,7 +2642,7 @@
       <c r="D104" s="66"/>
       <c r="E104" s="66"/>
       <c r="F104" s="66"/>
-      <c r="G104" s="51"/>
+      <c r="G104" s="49"/>
       <c r="H104" s="3" t="s">
         <v>109</v>
       </c>
@@ -2651,7 +2653,7 @@
       <c r="C105" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G105" s="51"/>
+      <c r="G105" s="49"/>
       <c r="H105" s="3" t="s">
         <v>70</v>
       </c>
@@ -2677,7 +2679,7 @@
     </row>
     <row r="108" spans="1:13">
       <c r="A108" s="17"/>
-      <c r="B108" s="55" t="s">
+      <c r="B108" s="53" t="s">
         <v>103</v>
       </c>
       <c r="C108" s="27"/>
@@ -2692,7 +2694,7 @@
     </row>
     <row r="109" spans="1:13">
       <c r="A109" s="17"/>
-      <c r="B109" s="56" t="s">
+      <c r="B109" s="54" t="s">
         <v>104</v>
       </c>
       <c r="C109" s="27"/>
@@ -2723,20 +2725,85 @@
       <c r="F115" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="119">
+  <mergeCells count="93">
+    <mergeCell ref="G74:H74"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="B77:E77"/>
+    <mergeCell ref="G77:H77"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="B44:H44"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="B72:H72"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="C104:F104"/>
+    <mergeCell ref="G79:H79"/>
+    <mergeCell ref="C102:G102"/>
+    <mergeCell ref="C100:G100"/>
+    <mergeCell ref="B89:F89"/>
+    <mergeCell ref="B90:F90"/>
+    <mergeCell ref="H102:I102"/>
+    <mergeCell ref="G81:H81"/>
+    <mergeCell ref="H101:I101"/>
+    <mergeCell ref="B88:E88"/>
+    <mergeCell ref="B83:K83"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="B38:M38"/>
+    <mergeCell ref="C101:G101"/>
+    <mergeCell ref="B71:E71"/>
+    <mergeCell ref="G71:H71"/>
+    <mergeCell ref="B79:E79"/>
+    <mergeCell ref="G80:H80"/>
+    <mergeCell ref="B80:E80"/>
+    <mergeCell ref="B69:H69"/>
+    <mergeCell ref="G76:H76"/>
+    <mergeCell ref="G89:H89"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="G70:H70"/>
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="B87:E87"/>
+    <mergeCell ref="L99:M99"/>
+    <mergeCell ref="B97:K97"/>
+    <mergeCell ref="J62:M62"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="H100:I100"/>
+    <mergeCell ref="B84:E84"/>
+    <mergeCell ref="B85:E85"/>
+    <mergeCell ref="B86:E86"/>
+    <mergeCell ref="B92:E92"/>
+    <mergeCell ref="B81:E81"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="B70:E70"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="G90:H90"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="B1:M1"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="B3:M3"/>
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="J7:L7"/>
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="B24:E24"/>
     <mergeCell ref="B7:D7"/>
@@ -2744,105 +2811,14 @@
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B6:C6"/>
     <mergeCell ref="B12:E12"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B13:E13"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="B23:E23"/>
     <mergeCell ref="B20:E20"/>
-    <mergeCell ref="G32:H32"/>
     <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="L99:M99"/>
-    <mergeCell ref="B97:K97"/>
-    <mergeCell ref="J62:M62"/>
-    <mergeCell ref="G73:H73"/>
-    <mergeCell ref="G86:H86"/>
-    <mergeCell ref="G85:H85"/>
-    <mergeCell ref="H100:I100"/>
-    <mergeCell ref="B84:E84"/>
-    <mergeCell ref="B85:E85"/>
-    <mergeCell ref="B86:E86"/>
-    <mergeCell ref="B92:E92"/>
-    <mergeCell ref="G93:H93"/>
-    <mergeCell ref="B81:E81"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="B70:E70"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="G90:H90"/>
-    <mergeCell ref="B76:F76"/>
-    <mergeCell ref="B88:E88"/>
-    <mergeCell ref="G78:H78"/>
-    <mergeCell ref="B77:E77"/>
-    <mergeCell ref="G77:H77"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="B38:M38"/>
-    <mergeCell ref="C101:G101"/>
-    <mergeCell ref="B71:E71"/>
-    <mergeCell ref="G71:H71"/>
-    <mergeCell ref="G95:H95"/>
-    <mergeCell ref="B79:E79"/>
-    <mergeCell ref="G80:H80"/>
-    <mergeCell ref="B56:H56"/>
-    <mergeCell ref="B80:E80"/>
-    <mergeCell ref="B69:H69"/>
-    <mergeCell ref="G76:H76"/>
-    <mergeCell ref="G94:H94"/>
-    <mergeCell ref="G89:H89"/>
-    <mergeCell ref="G65:H65"/>
-    <mergeCell ref="G70:H70"/>
-    <mergeCell ref="B60:E60"/>
-    <mergeCell ref="B87:E87"/>
-    <mergeCell ref="G74:H74"/>
-    <mergeCell ref="C104:F104"/>
-    <mergeCell ref="G79:H79"/>
-    <mergeCell ref="G84:H84"/>
-    <mergeCell ref="C102:G102"/>
-    <mergeCell ref="C100:G100"/>
-    <mergeCell ref="B89:F89"/>
-    <mergeCell ref="B90:F90"/>
-    <mergeCell ref="B93:F93"/>
-    <mergeCell ref="B94:F94"/>
-    <mergeCell ref="B95:F95"/>
-    <mergeCell ref="H102:I102"/>
-    <mergeCell ref="G81:H81"/>
-    <mergeCell ref="H101:I101"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="B83:K83"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B46:H46"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="B43:H43"/>
-    <mergeCell ref="B44:H44"/>
-    <mergeCell ref="G60:H60"/>
-    <mergeCell ref="B72:H72"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Further updates to blank PPF
</commit_message>
<xml_diff>
--- a/blankPPF.xlsx
+++ b/blankPPF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshpopp/Downloads/ppfproj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4482310-EB21-BC49-856D-2B95CC9D85DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0C79D9-E805-204C-B99F-6CCE74022DDB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1100" windowWidth="19500" windowHeight="14360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="113">
   <si>
     <t>PROGRAM PROGRESS FORM</t>
   </si>
@@ -313,9 +313,6 @@
   </si>
   <si>
     <t>Capstone Design Course</t>
-  </si>
-  <si>
-    <t>Laboratory Course</t>
   </si>
   <si>
     <r>
@@ -362,9 +359,6 @@
   </si>
   <si>
     <t>BEE 4500</t>
-  </si>
-  <si>
-    <t>CHEME 3130 or MSE 3030</t>
   </si>
   <si>
     <t xml:space="preserve">BEE 2220, ENGRD 2210, </t>
@@ -498,6 +492,12 @@
       </rPr>
       <t>6 credits</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">    CHEME 3130 or MSE 3030</t>
+  </si>
+  <si>
+    <t>Multivariable Calculus for Engineers*</t>
   </si>
 </sst>
 </file>
@@ -603,7 +603,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -717,6 +717,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1057,8 +1060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1114,7 +1117,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B3" s="52" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C3" s="41"/>
       <c r="D3" s="41"/>
@@ -1269,7 +1272,7 @@
       <c r="E12" s="36"/>
       <c r="F12" s="25"/>
       <c r="G12" s="39" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H12" s="39"/>
       <c r="I12" s="35"/>
@@ -1278,14 +1281,14 @@
     <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13" s="11"/>
       <c r="B13" s="39" t="s">
-        <v>16</v>
+        <v>112</v>
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="36"/>
       <c r="E13" s="36"/>
       <c r="F13" s="25"/>
       <c r="G13" s="39" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H13" s="39"/>
       <c r="I13" s="23"/>
@@ -1419,7 +1422,7 @@
       <c r="E23" s="36"/>
       <c r="F23" s="25"/>
       <c r="G23" s="36" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H23" s="36"/>
       <c r="I23" s="35"/>
@@ -1506,7 +1509,7 @@
     <row r="30" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A30" s="11"/>
       <c r="B30" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G30" s="25"/>
       <c r="H30" s="25"/>
@@ -1534,7 +1537,7 @@
     <row r="32" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A32" s="11"/>
       <c r="B32" s="25" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C32" s="25"/>
       <c r="D32" s="25"/>
@@ -1568,7 +1571,7 @@
         <v>22</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C34" s="25"/>
       <c r="D34" s="25"/>
@@ -2001,7 +2004,7 @@
         <v>24</v>
       </c>
       <c r="B64" s="41" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C64" s="36"/>
       <c r="D64" s="36"/>
@@ -2018,7 +2021,7 @@
       <c r="E65" s="36"/>
       <c r="F65" s="25"/>
       <c r="G65" s="36" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H65" s="36"/>
       <c r="I65" s="35"/>
@@ -2060,7 +2063,7 @@
         <v>25</v>
       </c>
       <c r="B68" s="24" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C68" s="25"/>
       <c r="D68" s="25"/>
@@ -2092,7 +2095,7 @@
       <c r="E70" s="36"/>
       <c r="F70" s="25"/>
       <c r="G70" s="36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H70" s="36"/>
       <c r="I70" s="35"/>
@@ -2108,7 +2111,7 @@
       <c r="E71" s="36"/>
       <c r="F71" s="25"/>
       <c r="G71" s="36" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H71" s="36"/>
       <c r="I71" s="23"/>
@@ -2117,7 +2120,7 @@
     <row r="72" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A72" s="3"/>
       <c r="B72" s="38" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C72" s="38"/>
       <c r="D72" s="38"/>
@@ -2131,14 +2134,14 @@
     <row r="73" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A73" s="11"/>
       <c r="B73" s="36" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C73" s="36"/>
       <c r="D73" s="36"/>
       <c r="E73" s="36"/>
       <c r="F73" s="25"/>
       <c r="G73" s="36" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H73" s="36"/>
       <c r="I73" s="35"/>
@@ -2154,11 +2157,11 @@
       <c r="E74" s="36"/>
       <c r="F74" s="25"/>
       <c r="G74" s="36" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H74" s="36"/>
-      <c r="I74" s="35"/>
-      <c r="K74" s="35"/>
+      <c r="I74" s="23"/>
+      <c r="K74" s="23"/>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A75" s="11"/>
@@ -2168,11 +2171,12 @@
       <c r="E75" s="25"/>
       <c r="F75" s="25"/>
       <c r="G75" s="25" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="H75" s="25"/>
-      <c r="I75" s="35"/>
-      <c r="K75" s="35"/>
+      <c r="I75" s="6"/>
+      <c r="J75" s="7"/>
+      <c r="K75" s="6"/>
     </row>
     <row r="76" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="11"/>
@@ -2184,24 +2188,24 @@
       <c r="E76" s="37"/>
       <c r="F76" s="37"/>
       <c r="G76" s="37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H76" s="37"/>
-      <c r="I76" s="23"/>
+      <c r="I76" s="35"/>
       <c r="J76" s="1"/>
-      <c r="K76" s="23"/>
+      <c r="K76" s="35"/>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A77" s="11"/>
       <c r="B77" s="36" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C77" s="36"/>
       <c r="D77" s="36"/>
       <c r="E77" s="36"/>
       <c r="F77" s="25"/>
       <c r="G77" s="36" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H77" s="36"/>
       <c r="I77" s="35"/>
@@ -2211,13 +2215,13 @@
     <row r="78" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A78" s="11"/>
       <c r="B78" s="30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D78" s="30"/>
       <c r="E78" s="30"/>
       <c r="F78" s="30"/>
       <c r="G78" s="37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H78" s="37"/>
       <c r="I78" s="35"/>
@@ -2243,14 +2247,14 @@
     <row r="80" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A80" s="11"/>
       <c r="B80" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C80" s="36"/>
       <c r="D80" s="36"/>
       <c r="E80" s="36"/>
       <c r="F80" s="25"/>
       <c r="G80" s="36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H80" s="36"/>
       <c r="I80" s="6"/>
@@ -2259,14 +2263,14 @@
     <row r="81" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A81" s="11"/>
       <c r="B81" s="36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C81" s="36"/>
       <c r="D81" s="36"/>
       <c r="E81" s="36"/>
       <c r="F81" s="25"/>
       <c r="G81" s="36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H81" s="36"/>
       <c r="I81" s="23"/>
@@ -2275,7 +2279,7 @@
     <row r="82" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A82" s="11"/>
       <c r="B82" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I82" s="34"/>
       <c r="J82" s="34"/>
@@ -2286,7 +2290,7 @@
     <row r="83" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A83" s="11"/>
       <c r="B83" s="36" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C83" s="36"/>
       <c r="D83" s="36"/>
@@ -2301,7 +2305,7 @@
     <row r="84" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A84" s="11"/>
       <c r="B84" s="36" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C84" s="36"/>
       <c r="D84" s="36"/>
@@ -2316,7 +2320,7 @@
     <row r="85" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A85" s="11"/>
       <c r="B85" s="36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C85" s="36"/>
       <c r="D85" s="36"/>
@@ -2330,7 +2334,7 @@
     <row r="86" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A86" s="11"/>
       <c r="B86" s="36" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C86" s="36"/>
       <c r="D86" s="36"/>
@@ -2344,7 +2348,7 @@
     <row r="87" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A87" s="11"/>
       <c r="B87" s="36" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C87" s="36"/>
       <c r="D87" s="36"/>
@@ -2358,7 +2362,7 @@
     <row r="88" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A88" s="11"/>
       <c r="B88" s="36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C88" s="36"/>
       <c r="D88" s="36"/>
@@ -2496,7 +2500,7 @@
       <c r="J99" s="29"/>
       <c r="K99" s="33"/>
       <c r="L99" s="42" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="M99" s="42"/>
     </row>
@@ -2528,19 +2532,25 @@
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A102" s="11"/>
-      <c r="B102" s="23"/>
-      <c r="C102" s="36" t="s">
-        <v>74</v>
-      </c>
+      <c r="B102" s="22"/>
+      <c r="C102" s="36"/>
       <c r="D102" s="36"/>
       <c r="E102" s="36"/>
       <c r="F102" s="36"/>
       <c r="G102" s="36"/>
-      <c r="H102" s="40"/>
-      <c r="I102" s="40"/>
+      <c r="H102" s="57"/>
+      <c r="I102" s="57"/>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A103" s="11"/>
+      <c r="B103" s="7"/>
+      <c r="C103" s="7"/>
+      <c r="D103" s="7"/>
+      <c r="E103" s="7"/>
+      <c r="F103" s="7"/>
+      <c r="G103" s="7"/>
+      <c r="H103" s="7"/>
+      <c r="I103" s="7"/>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A104" s="11"/>
@@ -2553,7 +2563,7 @@
       <c r="F104" s="39"/>
       <c r="G104" s="21"/>
       <c r="H104" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.15">
@@ -2574,19 +2584,19 @@
     <row r="107" spans="1:13" ht="15" x14ac:dyDescent="0.15">
       <c r="A107" s="11"/>
       <c r="B107" s="55" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A108" s="11"/>
       <c r="B108" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A109" s="11"/>
       <c r="B109" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Lots of updates in response to first round of critiques using the program for real PPFs
</commit_message>
<xml_diff>
--- a/blankPPF.xlsx
+++ b/blankPPF.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshpopp/Downloads/ppfproj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0C79D9-E805-204C-B99F-6CCE74022DDB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1014EAB-7852-2948-B4AC-7924FE8D94CA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1100" windowWidth="19500" windowHeight="14360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -463,19 +463,6 @@
   </si>
   <si>
     <r>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Engineering distribution requirement is satisfied by ENGRD 2020 and ENGRD 2600 or ENGRD 2510</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <b/>
         <sz val="10"/>
@@ -498,6 +485,19 @@
   </si>
   <si>
     <t>Multivariable Calculus for Engineers*</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Engineering distribution requirement is satisfied by ENGRD 2020 and ENGRD 2600 or ENGRD 2510</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -603,7 +603,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -672,22 +672,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -695,6 +696,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -709,14 +716,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1061,7 +1065,7 @@
   <dimension ref="A1:N115"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+      <selection activeCell="L5" sqref="L5:M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1082,134 +1086,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
       <c r="N1" s="12"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
       <c r="N2" s="2"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
       <c r="N3" s="2"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
       <c r="F5" s="26"/>
       <c r="G5" s="26"/>
       <c r="I5" s="25"/>
-      <c r="J5" s="41" t="s">
+      <c r="J5" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="41"/>
-      <c r="L5" s="53">
+      <c r="K5" s="44"/>
+      <c r="L5" s="46">
         <f ca="1">TODAY()</f>
-        <v>43678</v>
-      </c>
-      <c r="M5" s="53"/>
+        <v>43704</v>
+      </c>
+      <c r="M5" s="46"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="46" t="s">
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="41" t="s">
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="41"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="42"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
       <c r="I7" s="25"/>
-      <c r="J7" s="41" t="s">
+      <c r="J7" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="44"/>
       <c r="M7" s="14"/>
     </row>
     <row r="8" spans="1:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
       <c r="J8" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="K8" s="54"/>
+      <c r="K8" s="38"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A9" s="9"/>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="49"/>
+      <c r="C9" s="54"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -1227,10 +1231,10 @@
     </row>
     <row r="10" spans="1:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10"/>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="51"/>
+      <c r="C10" s="56"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -1254,75 +1258,75 @@
       <c r="A11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
       <c r="F11" s="26"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12" s="11"/>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
       <c r="F12" s="25"/>
-      <c r="G12" s="39" t="s">
+      <c r="G12" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="H12" s="39"/>
+      <c r="H12" s="43"/>
       <c r="I12" s="35"/>
       <c r="K12" s="35"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13" s="11"/>
-      <c r="B13" s="39" t="s">
-        <v>112</v>
-      </c>
-      <c r="C13" s="39"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
+      <c r="B13" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="43"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="39" t="s">
+      <c r="G13" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="H13" s="39"/>
+      <c r="H13" s="43"/>
       <c r="I13" s="23"/>
       <c r="K13" s="35"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14" s="11"/>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
       <c r="F14" s="25"/>
-      <c r="G14" s="39" t="s">
+      <c r="G14" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="H14" s="39"/>
+      <c r="H14" s="43"/>
       <c r="I14" s="23"/>
       <c r="K14" s="35"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A15" s="11"/>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="39"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
       <c r="F15" s="25"/>
-      <c r="G15" s="39" t="s">
+      <c r="G15" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="H15" s="39"/>
+      <c r="H15" s="43"/>
       <c r="I15" s="23"/>
       <c r="K15" s="35"/>
       <c r="M15" s="35">
@@ -1332,13 +1336,13 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A16" s="11"/>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A17" s="11"/>
@@ -1347,43 +1351,43 @@
       <c r="A18" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
       <c r="F18" s="25"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A19" s="11"/>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="36" t="s">
+      <c r="G19" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="H19" s="36"/>
+      <c r="H19" s="42"/>
       <c r="I19" s="35"/>
       <c r="K19" s="35"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A20" s="11"/>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
       <c r="F20" s="25"/>
-      <c r="G20" s="36" t="s">
+      <c r="G20" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="36"/>
+      <c r="H20" s="42"/>
       <c r="I20" s="35"/>
       <c r="K20" s="23"/>
       <c r="M20" s="35">
@@ -1399,12 +1403,12 @@
       <c r="A22" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
       <c r="F22" s="25"/>
       <c r="I22" s="6"/>
       <c r="J22" s="7"/>
@@ -1414,29 +1418,29 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A23" s="11"/>
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
       <c r="F23" s="25"/>
-      <c r="G23" s="36" t="s">
+      <c r="G23" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="H23" s="36"/>
+      <c r="H23" s="42"/>
       <c r="I23" s="35"/>
       <c r="K23" s="35"/>
       <c r="M23" s="6"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A24" s="11"/>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
       <c r="G24" s="25" t="s">
         <v>60</v>
       </c>
@@ -1571,7 +1575,7 @@
         <v>22</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C34" s="25"/>
       <c r="D34" s="25"/>
@@ -1624,20 +1628,20 @@
       <c r="A38" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="41" t="s">
+      <c r="B38" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36"/>
-      <c r="K38" s="36"/>
-      <c r="L38" s="36"/>
-      <c r="M38" s="36"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="42"/>
+      <c r="G38" s="42"/>
+      <c r="H38" s="42"/>
+      <c r="I38" s="42"/>
+      <c r="J38" s="42"/>
+      <c r="K38" s="42"/>
+      <c r="L38" s="42"/>
+      <c r="M38" s="42"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A39" s="11"/>
@@ -1673,29 +1677,29 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A41" s="11"/>
-      <c r="B41" s="37" t="s">
+      <c r="B41" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="C41" s="37"/>
-      <c r="D41" s="37"/>
-      <c r="E41" s="37"/>
-      <c r="F41" s="37"/>
-      <c r="G41" s="37"/>
-      <c r="H41" s="37"/>
+      <c r="C41" s="51"/>
+      <c r="D41" s="51"/>
+      <c r="E41" s="51"/>
+      <c r="F41" s="51"/>
+      <c r="G41" s="51"/>
+      <c r="H41" s="51"/>
       <c r="I41" s="6"/>
       <c r="K41" s="6"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A42" s="11"/>
-      <c r="B42" s="37" t="s">
+      <c r="B42" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="37"/>
-      <c r="D42" s="37"/>
-      <c r="E42" s="37"/>
-      <c r="F42" s="37"/>
-      <c r="G42" s="37"/>
-      <c r="H42" s="37"/>
+      <c r="C42" s="51"/>
+      <c r="D42" s="51"/>
+      <c r="E42" s="51"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="51"/>
+      <c r="H42" s="51"/>
       <c r="I42" s="6"/>
       <c r="J42" s="7"/>
       <c r="K42" s="6"/>
@@ -1703,15 +1707,15 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A43" s="11"/>
-      <c r="B43" s="37" t="s">
+      <c r="B43" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="37"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
-      <c r="G43" s="37"/>
-      <c r="H43" s="37"/>
+      <c r="C43" s="51"/>
+      <c r="D43" s="51"/>
+      <c r="E43" s="51"/>
+      <c r="F43" s="51"/>
+      <c r="G43" s="51"/>
+      <c r="H43" s="51"/>
       <c r="I43" s="7"/>
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
@@ -1719,15 +1723,15 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A44" s="11"/>
-      <c r="B44" s="37" t="s">
+      <c r="B44" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="C44" s="37"/>
-      <c r="D44" s="37"/>
-      <c r="E44" s="37"/>
-      <c r="F44" s="37"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="37"/>
+      <c r="C44" s="51"/>
+      <c r="D44" s="51"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="51"/>
+      <c r="H44" s="51"/>
       <c r="I44" s="7"/>
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
@@ -1735,15 +1739,15 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A45" s="11"/>
-      <c r="B45" s="37" t="s">
+      <c r="B45" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="37"/>
-      <c r="D45" s="37"/>
-      <c r="E45" s="37"/>
-      <c r="F45" s="37"/>
-      <c r="G45" s="37"/>
-      <c r="H45" s="37"/>
+      <c r="C45" s="51"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="51"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="51"/>
+      <c r="H45" s="51"/>
       <c r="I45" s="6"/>
       <c r="J45" s="7"/>
       <c r="K45" s="6"/>
@@ -1751,15 +1755,15 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A46" s="11"/>
-      <c r="B46" s="37" t="s">
+      <c r="B46" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="C46" s="37"/>
-      <c r="D46" s="37"/>
-      <c r="E46" s="37"/>
-      <c r="F46" s="37"/>
-      <c r="G46" s="37"/>
-      <c r="H46" s="37"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="51"/>
+      <c r="F46" s="51"/>
+      <c r="G46" s="51"/>
+      <c r="H46" s="51"/>
       <c r="I46" s="6"/>
       <c r="J46" s="7"/>
       <c r="K46" s="6"/>
@@ -1783,115 +1787,115 @@
       <c r="F48" s="25"/>
       <c r="G48" s="25"/>
       <c r="H48" s="25"/>
-      <c r="I48" s="6"/>
+      <c r="I48" s="41"/>
       <c r="J48" s="7"/>
-      <c r="K48" s="6"/>
+      <c r="K48" s="41"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A49" s="11"/>
-      <c r="B49" s="56"/>
-      <c r="C49" s="56"/>
-      <c r="D49" s="56"/>
-      <c r="E49" s="56"/>
-      <c r="F49" s="56"/>
-      <c r="G49" s="56"/>
-      <c r="H49" s="56"/>
-      <c r="I49" s="56"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="40"/>
+      <c r="D49" s="40"/>
+      <c r="E49" s="40"/>
+      <c r="F49" s="40"/>
+      <c r="G49" s="40"/>
+      <c r="H49" s="40"/>
+      <c r="I49" s="37"/>
       <c r="J49" s="26"/>
-      <c r="K49" s="56"/>
+      <c r="K49" s="37"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A50" s="11"/>
-      <c r="B50" s="56"/>
-      <c r="C50" s="56"/>
-      <c r="D50" s="56"/>
-      <c r="E50" s="56"/>
-      <c r="F50" s="56"/>
-      <c r="G50" s="56"/>
-      <c r="H50" s="56"/>
-      <c r="I50" s="56"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="40"/>
+      <c r="D50" s="40"/>
+      <c r="E50" s="40"/>
+      <c r="F50" s="40"/>
+      <c r="G50" s="40"/>
+      <c r="H50" s="40"/>
+      <c r="I50" s="37"/>
       <c r="J50" s="26"/>
-      <c r="K50" s="56"/>
+      <c r="K50" s="37"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A51" s="11"/>
-      <c r="B51" s="56"/>
-      <c r="C51" s="56"/>
-      <c r="D51" s="56"/>
-      <c r="E51" s="56"/>
-      <c r="F51" s="56"/>
-      <c r="G51" s="56"/>
-      <c r="H51" s="56"/>
-      <c r="I51" s="56"/>
+      <c r="B51" s="40"/>
+      <c r="C51" s="40"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="40"/>
+      <c r="F51" s="40"/>
+      <c r="G51" s="40"/>
+      <c r="H51" s="40"/>
+      <c r="I51" s="37"/>
       <c r="J51" s="26"/>
-      <c r="K51" s="56"/>
+      <c r="K51" s="37"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A52" s="11"/>
-      <c r="B52" s="56"/>
-      <c r="C52" s="56"/>
-      <c r="D52" s="56"/>
-      <c r="E52" s="56"/>
-      <c r="F52" s="56"/>
-      <c r="G52" s="56"/>
-      <c r="H52" s="56"/>
-      <c r="I52" s="56"/>
+      <c r="B52" s="40"/>
+      <c r="C52" s="40"/>
+      <c r="D52" s="40"/>
+      <c r="E52" s="40"/>
+      <c r="F52" s="40"/>
+      <c r="G52" s="40"/>
+      <c r="H52" s="40"/>
+      <c r="I52" s="37"/>
       <c r="J52" s="26"/>
-      <c r="K52" s="56"/>
+      <c r="K52" s="37"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A53" s="11"/>
-      <c r="B53" s="56"/>
-      <c r="C53" s="56"/>
-      <c r="D53" s="56"/>
-      <c r="E53" s="56"/>
-      <c r="F53" s="56"/>
-      <c r="G53" s="56"/>
-      <c r="H53" s="56"/>
-      <c r="I53" s="56"/>
+      <c r="B53" s="40"/>
+      <c r="C53" s="40"/>
+      <c r="D53" s="40"/>
+      <c r="E53" s="40"/>
+      <c r="F53" s="40"/>
+      <c r="G53" s="40"/>
+      <c r="H53" s="40"/>
+      <c r="I53" s="37"/>
       <c r="J53" s="26"/>
-      <c r="K53" s="56"/>
+      <c r="K53" s="37"/>
       <c r="M53" s="6"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A54" s="11"/>
-      <c r="B54" s="56"/>
-      <c r="C54" s="56"/>
-      <c r="D54" s="56"/>
-      <c r="E54" s="56"/>
-      <c r="F54" s="56"/>
-      <c r="G54" s="56"/>
-      <c r="H54" s="56"/>
-      <c r="I54" s="56"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="40"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="40"/>
+      <c r="F54" s="40"/>
+      <c r="G54" s="40"/>
+      <c r="H54" s="40"/>
+      <c r="I54" s="37"/>
       <c r="J54" s="26"/>
-      <c r="K54" s="56"/>
+      <c r="K54" s="37"/>
       <c r="M54" s="6"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A55" s="11"/>
-      <c r="B55" s="56"/>
-      <c r="C55" s="56"/>
-      <c r="D55" s="56"/>
-      <c r="E55" s="56"/>
-      <c r="F55" s="56"/>
-      <c r="G55" s="56"/>
-      <c r="H55" s="56"/>
-      <c r="I55" s="35"/>
-      <c r="K55" s="35"/>
+      <c r="B55" s="40"/>
+      <c r="C55" s="40"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="40"/>
+      <c r="F55" s="40"/>
+      <c r="G55" s="40"/>
+      <c r="H55" s="40"/>
+      <c r="I55" s="37"/>
+      <c r="K55" s="37"/>
       <c r="M55" s="6"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A56" s="11"/>
-      <c r="B56" s="56"/>
-      <c r="C56" s="56"/>
-      <c r="D56" s="56"/>
-      <c r="E56" s="56"/>
-      <c r="F56" s="56"/>
-      <c r="G56" s="56"/>
-      <c r="H56" s="56"/>
-      <c r="I56" s="35"/>
+      <c r="B56" s="40"/>
+      <c r="C56" s="40"/>
+      <c r="D56" s="40"/>
+      <c r="E56" s="40"/>
+      <c r="F56" s="40"/>
+      <c r="G56" s="40"/>
+      <c r="H56" s="40"/>
+      <c r="I56" s="37"/>
       <c r="J56" s="7"/>
-      <c r="K56" s="35"/>
+      <c r="K56" s="37"/>
       <c r="L56" s="7"/>
       <c r="M56" s="6"/>
     </row>
@@ -1976,13 +1980,13 @@
       <c r="I62" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="J62" s="43">
+      <c r="J62" s="57">
         <f>B5</f>
         <v>0</v>
       </c>
-      <c r="K62" s="43"/>
-      <c r="L62" s="43"/>
-      <c r="M62" s="43"/>
+      <c r="K62" s="57"/>
+      <c r="L62" s="57"/>
+      <c r="M62" s="57"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A63" s="11"/>
@@ -2003,27 +2007,27 @@
       <c r="A64" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B64" s="41" t="s">
+      <c r="B64" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="C64" s="36"/>
-      <c r="D64" s="36"/>
-      <c r="E64" s="36"/>
+      <c r="C64" s="42"/>
+      <c r="D64" s="42"/>
+      <c r="E64" s="42"/>
       <c r="F64" s="25"/>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A65" s="11"/>
-      <c r="B65" s="36" t="s">
+      <c r="B65" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="C65" s="36"/>
-      <c r="D65" s="36"/>
-      <c r="E65" s="36"/>
+      <c r="C65" s="42"/>
+      <c r="D65" s="42"/>
+      <c r="E65" s="42"/>
       <c r="F65" s="25"/>
-      <c r="G65" s="36" t="s">
+      <c r="G65" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="H65" s="36"/>
+      <c r="H65" s="42"/>
       <c r="I65" s="35"/>
       <c r="K65" s="35"/>
       <c r="M65" s="35">
@@ -2038,8 +2042,8 @@
       <c r="D66" s="25"/>
       <c r="E66" s="25"/>
       <c r="F66" s="25"/>
-      <c r="G66" s="36"/>
-      <c r="H66" s="36"/>
+      <c r="G66" s="42"/>
+      <c r="H66" s="42"/>
       <c r="I66" s="22"/>
       <c r="K66" s="22"/>
     </row>
@@ -2073,93 +2077,93 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A69" s="11"/>
-      <c r="B69" s="38" t="s">
+      <c r="B69" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="C69" s="38"/>
-      <c r="D69" s="38"/>
-      <c r="E69" s="38"/>
-      <c r="F69" s="38"/>
-      <c r="G69" s="38"/>
-      <c r="H69" s="38"/>
+      <c r="C69" s="58"/>
+      <c r="D69" s="58"/>
+      <c r="E69" s="58"/>
+      <c r="F69" s="58"/>
+      <c r="G69" s="58"/>
+      <c r="H69" s="58"/>
       <c r="I69" s="7"/>
       <c r="K69" s="7"/>
     </row>
     <row r="70" spans="1:13" ht="15" x14ac:dyDescent="0.15">
       <c r="A70" s="11"/>
-      <c r="B70" s="36" t="s">
+      <c r="B70" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="C70" s="36"/>
-      <c r="D70" s="36"/>
-      <c r="E70" s="36"/>
+      <c r="C70" s="42"/>
+      <c r="D70" s="42"/>
+      <c r="E70" s="42"/>
       <c r="F70" s="25"/>
-      <c r="G70" s="36" t="s">
+      <c r="G70" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="H70" s="36"/>
+      <c r="H70" s="42"/>
       <c r="I70" s="35"/>
       <c r="K70" s="35"/>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A71" s="11"/>
-      <c r="B71" s="36" t="s">
+      <c r="B71" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="C71" s="36"/>
-      <c r="D71" s="36"/>
-      <c r="E71" s="36"/>
+      <c r="C71" s="42"/>
+      <c r="D71" s="42"/>
+      <c r="E71" s="42"/>
       <c r="F71" s="25"/>
-      <c r="G71" s="36" t="s">
+      <c r="G71" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="H71" s="36"/>
+      <c r="H71" s="42"/>
       <c r="I71" s="23"/>
       <c r="K71" s="23"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A72" s="3"/>
-      <c r="B72" s="38" t="s">
+      <c r="B72" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="C72" s="38"/>
-      <c r="D72" s="38"/>
-      <c r="E72" s="38"/>
-      <c r="F72" s="38"/>
-      <c r="G72" s="38"/>
-      <c r="H72" s="38"/>
+      <c r="C72" s="58"/>
+      <c r="D72" s="58"/>
+      <c r="E72" s="58"/>
+      <c r="F72" s="58"/>
+      <c r="G72" s="58"/>
+      <c r="H72" s="58"/>
       <c r="I72" s="7"/>
       <c r="K72" s="7"/>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A73" s="11"/>
-      <c r="B73" s="36" t="s">
+      <c r="B73" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="C73" s="36"/>
-      <c r="D73" s="36"/>
-      <c r="E73" s="36"/>
+      <c r="C73" s="42"/>
+      <c r="D73" s="42"/>
+      <c r="E73" s="42"/>
       <c r="F73" s="25"/>
-      <c r="G73" s="36" t="s">
+      <c r="G73" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="H73" s="36"/>
+      <c r="H73" s="42"/>
       <c r="I73" s="35"/>
       <c r="K73" s="35"/>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A74" s="11"/>
-      <c r="B74" s="36" t="s">
+      <c r="B74" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C74" s="36"/>
-      <c r="D74" s="36"/>
-      <c r="E74" s="36"/>
+      <c r="C74" s="42"/>
+      <c r="D74" s="42"/>
+      <c r="E74" s="42"/>
       <c r="F74" s="25"/>
-      <c r="G74" s="36" t="s">
+      <c r="G74" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="H74" s="36"/>
+      <c r="H74" s="42"/>
       <c r="I74" s="23"/>
       <c r="K74" s="23"/>
     </row>
@@ -2171,7 +2175,7 @@
       <c r="E75" s="25"/>
       <c r="F75" s="25"/>
       <c r="G75" s="25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H75" s="25"/>
       <c r="I75" s="6"/>
@@ -2180,34 +2184,34 @@
     </row>
     <row r="76" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="11"/>
-      <c r="B76" s="37" t="s">
+      <c r="B76" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="C76" s="37"/>
-      <c r="D76" s="37"/>
-      <c r="E76" s="37"/>
-      <c r="F76" s="37"/>
-      <c r="G76" s="37" t="s">
+      <c r="C76" s="51"/>
+      <c r="D76" s="51"/>
+      <c r="E76" s="51"/>
+      <c r="F76" s="51"/>
+      <c r="G76" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="H76" s="37"/>
+      <c r="H76" s="51"/>
       <c r="I76" s="35"/>
       <c r="J76" s="1"/>
       <c r="K76" s="35"/>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A77" s="11"/>
-      <c r="B77" s="36" t="s">
+      <c r="B77" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="C77" s="36"/>
-      <c r="D77" s="36"/>
-      <c r="E77" s="36"/>
+      <c r="C77" s="42"/>
+      <c r="D77" s="42"/>
+      <c r="E77" s="42"/>
       <c r="F77" s="25"/>
-      <c r="G77" s="36" t="s">
+      <c r="G77" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="H77" s="36"/>
+      <c r="H77" s="42"/>
       <c r="I77" s="35"/>
       <c r="J77" s="1"/>
       <c r="K77" s="35"/>
@@ -2220,59 +2224,59 @@
       <c r="D78" s="30"/>
       <c r="E78" s="30"/>
       <c r="F78" s="30"/>
-      <c r="G78" s="37" t="s">
+      <c r="G78" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="H78" s="37"/>
+      <c r="H78" s="51"/>
       <c r="I78" s="35"/>
       <c r="J78" s="1"/>
       <c r="K78" s="35"/>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A79" s="11"/>
-      <c r="B79" s="36" t="s">
+      <c r="B79" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="C79" s="36"/>
-      <c r="D79" s="36"/>
-      <c r="E79" s="36"/>
+      <c r="C79" s="42"/>
+      <c r="D79" s="42"/>
+      <c r="E79" s="42"/>
       <c r="F79" s="25"/>
-      <c r="G79" s="36" t="s">
+      <c r="G79" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="H79" s="36"/>
+      <c r="H79" s="42"/>
       <c r="I79" s="35"/>
       <c r="K79" s="35"/>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A80" s="11"/>
-      <c r="B80" s="36" t="s">
+      <c r="B80" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="C80" s="36"/>
-      <c r="D80" s="36"/>
-      <c r="E80" s="36"/>
+      <c r="C80" s="42"/>
+      <c r="D80" s="42"/>
+      <c r="E80" s="42"/>
       <c r="F80" s="25"/>
-      <c r="G80" s="36" t="s">
+      <c r="G80" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="H80" s="36"/>
+      <c r="H80" s="42"/>
       <c r="I80" s="6"/>
       <c r="K80" s="6"/>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A81" s="11"/>
-      <c r="B81" s="36" t="s">
+      <c r="B81" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="C81" s="36"/>
-      <c r="D81" s="36"/>
-      <c r="E81" s="36"/>
+      <c r="C81" s="42"/>
+      <c r="D81" s="42"/>
+      <c r="E81" s="42"/>
       <c r="F81" s="25"/>
-      <c r="G81" s="36" t="s">
+      <c r="G81" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="H81" s="36"/>
+      <c r="H81" s="42"/>
       <c r="I81" s="23"/>
       <c r="K81" s="23"/>
     </row>
@@ -2289,27 +2293,27 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A83" s="11"/>
-      <c r="B83" s="36" t="s">
+      <c r="B83" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="C83" s="36"/>
-      <c r="D83" s="36"/>
-      <c r="E83" s="36"/>
-      <c r="F83" s="36"/>
-      <c r="G83" s="36"/>
-      <c r="H83" s="36"/>
-      <c r="I83" s="36"/>
-      <c r="J83" s="36"/>
-      <c r="K83" s="36"/>
+      <c r="C83" s="42"/>
+      <c r="D83" s="42"/>
+      <c r="E83" s="42"/>
+      <c r="F83" s="42"/>
+      <c r="G83" s="42"/>
+      <c r="H83" s="42"/>
+      <c r="I83" s="42"/>
+      <c r="J83" s="42"/>
+      <c r="K83" s="42"/>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A84" s="11"/>
-      <c r="B84" s="36" t="s">
+      <c r="B84" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="C84" s="36"/>
-      <c r="D84" s="36"/>
-      <c r="E84" s="36"/>
+      <c r="C84" s="42"/>
+      <c r="D84" s="42"/>
+      <c r="E84" s="42"/>
       <c r="F84" s="25"/>
       <c r="G84" s="25"/>
       <c r="H84" s="25"/>
@@ -2319,12 +2323,12 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A85" s="11"/>
-      <c r="B85" s="36" t="s">
+      <c r="B85" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="C85" s="36"/>
-      <c r="D85" s="36"/>
-      <c r="E85" s="36"/>
+      <c r="C85" s="42"/>
+      <c r="D85" s="42"/>
+      <c r="E85" s="42"/>
       <c r="F85" s="25"/>
       <c r="G85" s="25"/>
       <c r="H85" s="25"/>
@@ -2333,12 +2337,12 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A86" s="11"/>
-      <c r="B86" s="36" t="s">
+      <c r="B86" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="C86" s="36"/>
-      <c r="D86" s="36"/>
-      <c r="E86" s="36"/>
+      <c r="C86" s="42"/>
+      <c r="D86" s="42"/>
+      <c r="E86" s="42"/>
       <c r="F86" s="25"/>
       <c r="G86" s="25"/>
       <c r="H86" s="25"/>
@@ -2347,12 +2351,12 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A87" s="11"/>
-      <c r="B87" s="36" t="s">
+      <c r="B87" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="C87" s="36"/>
-      <c r="D87" s="36"/>
-      <c r="E87" s="36"/>
+      <c r="C87" s="42"/>
+      <c r="D87" s="42"/>
+      <c r="E87" s="42"/>
       <c r="F87" s="25"/>
       <c r="G87" s="25"/>
       <c r="H87" s="25"/>
@@ -2361,12 +2365,12 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A88" s="11"/>
-      <c r="B88" s="36" t="s">
+      <c r="B88" s="42" t="s">
         <v>88</v>
       </c>
-      <c r="C88" s="36"/>
-      <c r="D88" s="36"/>
-      <c r="E88" s="36"/>
+      <c r="C88" s="42"/>
+      <c r="D88" s="42"/>
+      <c r="E88" s="42"/>
       <c r="F88" s="25"/>
       <c r="G88" s="25"/>
       <c r="H88" s="25"/>
@@ -2408,12 +2412,12 @@
       <c r="A92" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B92" s="41" t="s">
+      <c r="B92" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="C92" s="36"/>
-      <c r="D92" s="36"/>
-      <c r="E92" s="36"/>
+      <c r="C92" s="42"/>
+      <c r="D92" s="42"/>
+      <c r="E92" s="42"/>
       <c r="F92" s="25"/>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.15">
@@ -2471,16 +2475,16 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A97" s="11"/>
-      <c r="B97" s="36"/>
-      <c r="C97" s="36"/>
-      <c r="D97" s="36"/>
-      <c r="E97" s="36"/>
-      <c r="F97" s="36"/>
-      <c r="G97" s="36"/>
-      <c r="H97" s="36"/>
-      <c r="I97" s="36"/>
-      <c r="J97" s="36"/>
-      <c r="K97" s="36"/>
+      <c r="B97" s="42"/>
+      <c r="C97" s="42"/>
+      <c r="D97" s="42"/>
+      <c r="E97" s="42"/>
+      <c r="F97" s="42"/>
+      <c r="G97" s="42"/>
+      <c r="H97" s="42"/>
+      <c r="I97" s="42"/>
+      <c r="J97" s="42"/>
+      <c r="K97" s="42"/>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A98" s="11"/>
@@ -2499,47 +2503,47 @@
       <c r="A99" s="11"/>
       <c r="J99" s="29"/>
       <c r="K99" s="33"/>
-      <c r="L99" s="42" t="s">
+      <c r="L99" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="M99" s="42"/>
+      <c r="M99" s="50"/>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A100" s="11"/>
       <c r="B100" s="35"/>
-      <c r="C100" s="36" t="s">
+      <c r="C100" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="D100" s="36"/>
-      <c r="E100" s="36"/>
-      <c r="F100" s="36"/>
-      <c r="G100" s="36"/>
-      <c r="H100" s="40"/>
-      <c r="I100" s="40"/>
+      <c r="D100" s="42"/>
+      <c r="E100" s="42"/>
+      <c r="F100" s="42"/>
+      <c r="G100" s="42"/>
+      <c r="H100" s="37"/>
+      <c r="I100" s="36"/>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A101" s="11"/>
       <c r="B101" s="23"/>
-      <c r="C101" s="36" t="s">
+      <c r="C101" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="D101" s="36"/>
-      <c r="E101" s="36"/>
-      <c r="F101" s="36"/>
-      <c r="G101" s="36"/>
-      <c r="H101" s="40"/>
-      <c r="I101" s="40"/>
+      <c r="D101" s="42"/>
+      <c r="E101" s="42"/>
+      <c r="F101" s="42"/>
+      <c r="G101" s="42"/>
+      <c r="H101" s="37"/>
+      <c r="I101" s="36"/>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A102" s="11"/>
       <c r="B102" s="22"/>
-      <c r="C102" s="36"/>
-      <c r="D102" s="36"/>
-      <c r="E102" s="36"/>
-      <c r="F102" s="36"/>
-      <c r="G102" s="36"/>
-      <c r="H102" s="57"/>
-      <c r="I102" s="57"/>
+      <c r="C102" s="42"/>
+      <c r="D102" s="42"/>
+      <c r="E102" s="42"/>
+      <c r="F102" s="42"/>
+      <c r="G102" s="42"/>
+      <c r="H102" s="59"/>
+      <c r="I102" s="59"/>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A103" s="11"/>
@@ -2555,12 +2559,12 @@
     <row r="104" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A104" s="11"/>
       <c r="B104" s="35"/>
-      <c r="C104" s="39" t="s">
+      <c r="C104" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="D104" s="39"/>
-      <c r="E104" s="39"/>
-      <c r="F104" s="39"/>
+      <c r="D104" s="43"/>
+      <c r="E104" s="43"/>
+      <c r="F104" s="43"/>
       <c r="G104" s="21"/>
       <c r="H104" s="3" t="s">
         <v>104</v>
@@ -2583,8 +2587,8 @@
     </row>
     <row r="107" spans="1:13" ht="15" x14ac:dyDescent="0.15">
       <c r="A107" s="11"/>
-      <c r="B107" s="55" t="s">
-        <v>109</v>
+      <c r="B107" s="39" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.15">
@@ -2617,7 +2621,74 @@
       <c r="F115" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="85">
+  <mergeCells count="83">
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="G74:H74"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="B77:E77"/>
+    <mergeCell ref="G77:H77"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="C104:F104"/>
+    <mergeCell ref="G79:H79"/>
+    <mergeCell ref="C102:G102"/>
+    <mergeCell ref="C100:G100"/>
+    <mergeCell ref="H102:I102"/>
+    <mergeCell ref="G81:H81"/>
+    <mergeCell ref="B88:E88"/>
+    <mergeCell ref="B83:K83"/>
+    <mergeCell ref="B38:M38"/>
+    <mergeCell ref="C101:G101"/>
+    <mergeCell ref="B71:E71"/>
+    <mergeCell ref="G71:H71"/>
+    <mergeCell ref="B79:E79"/>
+    <mergeCell ref="G80:H80"/>
+    <mergeCell ref="B80:E80"/>
+    <mergeCell ref="B69:H69"/>
+    <mergeCell ref="G76:H76"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="G70:H70"/>
+    <mergeCell ref="B87:E87"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="B44:H44"/>
+    <mergeCell ref="B72:H72"/>
+    <mergeCell ref="B84:E84"/>
+    <mergeCell ref="B85:E85"/>
+    <mergeCell ref="B86:E86"/>
+    <mergeCell ref="B92:E92"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="L99:M99"/>
+    <mergeCell ref="B97:K97"/>
+    <mergeCell ref="J62:M62"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="B81:E81"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="B70:E70"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="J5:K5"/>
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="B24:E24"/>
     <mergeCell ref="B7:D7"/>
@@ -2633,76 +2704,7 @@
     <mergeCell ref="B23:E23"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B1:M1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="J7:L7"/>
     <mergeCell ref="B19:E19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="L99:M99"/>
-    <mergeCell ref="B97:K97"/>
-    <mergeCell ref="J62:M62"/>
-    <mergeCell ref="G73:H73"/>
-    <mergeCell ref="H100:I100"/>
-    <mergeCell ref="B84:E84"/>
-    <mergeCell ref="B85:E85"/>
-    <mergeCell ref="B86:E86"/>
-    <mergeCell ref="B92:E92"/>
-    <mergeCell ref="B81:E81"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="B70:E70"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="B76:F76"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B38:M38"/>
-    <mergeCell ref="C101:G101"/>
-    <mergeCell ref="B71:E71"/>
-    <mergeCell ref="G71:H71"/>
-    <mergeCell ref="B79:E79"/>
-    <mergeCell ref="G80:H80"/>
-    <mergeCell ref="B80:E80"/>
-    <mergeCell ref="B69:H69"/>
-    <mergeCell ref="G76:H76"/>
-    <mergeCell ref="G65:H65"/>
-    <mergeCell ref="G70:H70"/>
-    <mergeCell ref="B87:E87"/>
-    <mergeCell ref="C104:F104"/>
-    <mergeCell ref="G79:H79"/>
-    <mergeCell ref="C102:G102"/>
-    <mergeCell ref="C100:G100"/>
-    <mergeCell ref="H102:I102"/>
-    <mergeCell ref="G81:H81"/>
-    <mergeCell ref="H101:I101"/>
-    <mergeCell ref="B88:E88"/>
-    <mergeCell ref="B83:K83"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="B43:H43"/>
-    <mergeCell ref="B44:H44"/>
-    <mergeCell ref="B72:H72"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="B46:H46"/>
-    <mergeCell ref="G74:H74"/>
-    <mergeCell ref="G78:H78"/>
-    <mergeCell ref="B77:E77"/>
-    <mergeCell ref="G77:H77"/>
-    <mergeCell ref="B74:E74"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
December questions from Brenda, part 1
</commit_message>
<xml_diff>
--- a/blankPPF.xlsx
+++ b/blankPPF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshpopp/Downloads/ppfproj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1014EAB-7852-2948-B4AC-7924FE8D94CA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF89016-B7BA-AF49-95BB-5226D298993E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1100" windowWidth="19500" windowHeight="14360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6660" yWindow="920" windowWidth="19500" windowHeight="14360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PPF 2007" sheetId="1" r:id="rId1"/>
@@ -487,17 +487,7 @@
     <t>Multivariable Calculus for Engineers*</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Engineering distribution requirement is satisfied by ENGRD 2020 and ENGRD 2600 or ENGRD 2510</t>
-    </r>
+    <t>a) Engineering distribution requirement is satisfied by ENGRD 2020 and ENGRD 2600 or ENGRD 2510</t>
   </si>
 </sst>
 </file>
@@ -603,7 +593,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -677,18 +667,26 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -696,12 +694,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -716,13 +708,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1064,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5:M5"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K31" activeCellId="1" sqref="I31 K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1086,54 +1075,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
       <c r="N1" s="12"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
       <c r="N2" s="2"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
       <c r="N3" s="2"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.15">
@@ -1141,21 +1130,21 @@
         <v>11</v>
       </c>
       <c r="B5" s="43"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
       <c r="F5" s="26"/>
       <c r="G5" s="26"/>
       <c r="I5" s="25"/>
-      <c r="J5" s="44" t="s">
+      <c r="J5" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="44"/>
-      <c r="L5" s="46">
+      <c r="K5" s="45"/>
+      <c r="L5" s="58">
         <f ca="1">TODAY()</f>
-        <v>43704</v>
-      </c>
-      <c r="M5" s="46"/>
+        <v>43816</v>
+      </c>
+      <c r="M5" s="58"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6" s="34" t="s">
@@ -1163,20 +1152,20 @@
       </c>
       <c r="B6" s="43"/>
       <c r="C6" s="43"/>
-      <c r="D6" s="49" t="s">
+      <c r="D6" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="44" t="s">
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="44"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="42"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7" s="24" t="s">
@@ -1185,15 +1174,15 @@
       <c r="B7" s="43"/>
       <c r="C7" s="43"/>
       <c r="D7" s="43"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
       <c r="I7" s="25"/>
-      <c r="J7" s="44" t="s">
+      <c r="J7" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="K7" s="44"/>
-      <c r="L7" s="44"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="45"/>
       <c r="M7" s="14"/>
     </row>
     <row r="8" spans="1:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
@@ -1258,12 +1247,12 @@
       <c r="A11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
       <c r="F11" s="26"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.15">
@@ -1272,8 +1261,8 @@
         <v>16</v>
       </c>
       <c r="C12" s="43"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="25"/>
       <c r="G12" s="43" t="s">
         <v>94</v>
@@ -1288,8 +1277,8 @@
         <v>111</v>
       </c>
       <c r="C13" s="43"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
       <c r="F13" s="25"/>
       <c r="G13" s="43" t="s">
         <v>95</v>
@@ -1304,8 +1293,8 @@
         <v>38</v>
       </c>
       <c r="C14" s="43"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
       <c r="F14" s="25"/>
       <c r="G14" s="43" t="s">
         <v>51</v>
@@ -1320,8 +1309,8 @@
         <v>39</v>
       </c>
       <c r="C15" s="43"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
       <c r="F15" s="25"/>
       <c r="G15" s="43" t="s">
         <v>52</v>
@@ -1336,13 +1325,13 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A16" s="11"/>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A17" s="11"/>
@@ -1351,43 +1340,43 @@
       <c r="A18" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
       <c r="F18" s="25"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A19" s="11"/>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="42" t="s">
+      <c r="G19" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="H19" s="42"/>
+      <c r="H19" s="41"/>
       <c r="I19" s="35"/>
       <c r="K19" s="35"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A20" s="11"/>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
       <c r="F20" s="25"/>
-      <c r="G20" s="42" t="s">
+      <c r="G20" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="42"/>
+      <c r="H20" s="41"/>
       <c r="I20" s="35"/>
       <c r="K20" s="23"/>
       <c r="M20" s="35">
@@ -1403,12 +1392,12 @@
       <c r="A22" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="44" t="s">
+      <c r="B22" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
       <c r="F22" s="25"/>
       <c r="I22" s="6"/>
       <c r="J22" s="7"/>
@@ -1418,29 +1407,29 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A23" s="11"/>
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
       <c r="F23" s="25"/>
-      <c r="G23" s="42" t="s">
+      <c r="G23" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="H23" s="42"/>
+      <c r="H23" s="41"/>
       <c r="I23" s="35"/>
       <c r="K23" s="35"/>
       <c r="M23" s="6"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A24" s="11"/>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
       <c r="G24" s="25" t="s">
         <v>60</v>
       </c>
@@ -1532,9 +1521,9 @@
       <c r="F31" s="25"/>
       <c r="G31" s="25"/>
       <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
+      <c r="I31" s="23"/>
       <c r="J31" s="25"/>
-      <c r="K31" s="25"/>
+      <c r="K31" s="23"/>
       <c r="L31" s="25"/>
       <c r="M31" s="25"/>
     </row>
@@ -1628,20 +1617,20 @@
       <c r="A38" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="44" t="s">
+      <c r="B38" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="42"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="42"/>
-      <c r="F38" s="42"/>
-      <c r="G38" s="42"/>
-      <c r="H38" s="42"/>
-      <c r="I38" s="42"/>
-      <c r="J38" s="42"/>
-      <c r="K38" s="42"/>
-      <c r="L38" s="42"/>
-      <c r="M38" s="42"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="41"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="41"/>
+      <c r="J38" s="41"/>
+      <c r="K38" s="41"/>
+      <c r="L38" s="41"/>
+      <c r="M38" s="41"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A39" s="11"/>
@@ -1677,29 +1666,29 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A41" s="11"/>
-      <c r="B41" s="51" t="s">
+      <c r="B41" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="C41" s="51"/>
-      <c r="D41" s="51"/>
-      <c r="E41" s="51"/>
-      <c r="F41" s="51"/>
-      <c r="G41" s="51"/>
-      <c r="H41" s="51"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="42"/>
+      <c r="H41" s="42"/>
       <c r="I41" s="6"/>
       <c r="K41" s="6"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A42" s="11"/>
-      <c r="B42" s="51" t="s">
+      <c r="B42" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="51"/>
-      <c r="D42" s="51"/>
-      <c r="E42" s="51"/>
-      <c r="F42" s="51"/>
-      <c r="G42" s="51"/>
-      <c r="H42" s="51"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="42"/>
+      <c r="H42" s="42"/>
       <c r="I42" s="6"/>
       <c r="J42" s="7"/>
       <c r="K42" s="6"/>
@@ -1707,15 +1696,15 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A43" s="11"/>
-      <c r="B43" s="51" t="s">
+      <c r="B43" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="51"/>
-      <c r="D43" s="51"/>
-      <c r="E43" s="51"/>
-      <c r="F43" s="51"/>
-      <c r="G43" s="51"/>
-      <c r="H43" s="51"/>
+      <c r="C43" s="42"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="42"/>
+      <c r="H43" s="42"/>
       <c r="I43" s="7"/>
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
@@ -1723,15 +1712,15 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A44" s="11"/>
-      <c r="B44" s="51" t="s">
+      <c r="B44" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="C44" s="51"/>
-      <c r="D44" s="51"/>
-      <c r="E44" s="51"/>
-      <c r="F44" s="51"/>
-      <c r="G44" s="51"/>
-      <c r="H44" s="51"/>
+      <c r="C44" s="42"/>
+      <c r="D44" s="42"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="42"/>
+      <c r="G44" s="42"/>
+      <c r="H44" s="42"/>
       <c r="I44" s="7"/>
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
@@ -1739,15 +1728,15 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A45" s="11"/>
-      <c r="B45" s="51" t="s">
+      <c r="B45" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="51"/>
-      <c r="D45" s="51"/>
-      <c r="E45" s="51"/>
-      <c r="F45" s="51"/>
-      <c r="G45" s="51"/>
-      <c r="H45" s="51"/>
+      <c r="C45" s="42"/>
+      <c r="D45" s="42"/>
+      <c r="E45" s="42"/>
+      <c r="F45" s="42"/>
+      <c r="G45" s="42"/>
+      <c r="H45" s="42"/>
       <c r="I45" s="6"/>
       <c r="J45" s="7"/>
       <c r="K45" s="6"/>
@@ -1755,15 +1744,15 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A46" s="11"/>
-      <c r="B46" s="51" t="s">
+      <c r="B46" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="C46" s="51"/>
-      <c r="D46" s="51"/>
-      <c r="E46" s="51"/>
-      <c r="F46" s="51"/>
-      <c r="G46" s="51"/>
-      <c r="H46" s="51"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="42"/>
+      <c r="E46" s="42"/>
+      <c r="F46" s="42"/>
+      <c r="G46" s="42"/>
+      <c r="H46" s="42"/>
       <c r="I46" s="6"/>
       <c r="J46" s="7"/>
       <c r="K46" s="6"/>
@@ -1787,71 +1776,71 @@
       <c r="F48" s="25"/>
       <c r="G48" s="25"/>
       <c r="H48" s="25"/>
-      <c r="I48" s="41"/>
+      <c r="I48" s="40"/>
       <c r="J48" s="7"/>
-      <c r="K48" s="41"/>
+      <c r="K48" s="40"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A49" s="11"/>
-      <c r="B49" s="40"/>
-      <c r="C49" s="40"/>
-      <c r="D49" s="40"/>
-      <c r="E49" s="40"/>
-      <c r="F49" s="40"/>
-      <c r="G49" s="40"/>
-      <c r="H49" s="40"/>
+      <c r="B49" s="39"/>
+      <c r="C49" s="39"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="39"/>
+      <c r="F49" s="39"/>
+      <c r="G49" s="39"/>
+      <c r="H49" s="37"/>
       <c r="I49" s="37"/>
       <c r="J49" s="26"/>
       <c r="K49" s="37"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A50" s="11"/>
-      <c r="B50" s="40"/>
-      <c r="C50" s="40"/>
-      <c r="D50" s="40"/>
-      <c r="E50" s="40"/>
-      <c r="F50" s="40"/>
-      <c r="G50" s="40"/>
-      <c r="H50" s="40"/>
+      <c r="B50" s="39"/>
+      <c r="C50" s="39"/>
+      <c r="D50" s="39"/>
+      <c r="E50" s="39"/>
+      <c r="F50" s="39"/>
+      <c r="G50" s="39"/>
+      <c r="H50" s="37"/>
       <c r="I50" s="37"/>
       <c r="J50" s="26"/>
       <c r="K50" s="37"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A51" s="11"/>
-      <c r="B51" s="40"/>
-      <c r="C51" s="40"/>
-      <c r="D51" s="40"/>
-      <c r="E51" s="40"/>
-      <c r="F51" s="40"/>
-      <c r="G51" s="40"/>
-      <c r="H51" s="40"/>
+      <c r="B51" s="39"/>
+      <c r="C51" s="39"/>
+      <c r="D51" s="39"/>
+      <c r="E51" s="39"/>
+      <c r="F51" s="39"/>
+      <c r="G51" s="39"/>
+      <c r="H51" s="37"/>
       <c r="I51" s="37"/>
       <c r="J51" s="26"/>
       <c r="K51" s="37"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A52" s="11"/>
-      <c r="B52" s="40"/>
-      <c r="C52" s="40"/>
-      <c r="D52" s="40"/>
-      <c r="E52" s="40"/>
-      <c r="F52" s="40"/>
-      <c r="G52" s="40"/>
-      <c r="H52" s="40"/>
+      <c r="B52" s="39"/>
+      <c r="C52" s="39"/>
+      <c r="D52" s="39"/>
+      <c r="E52" s="39"/>
+      <c r="F52" s="39"/>
+      <c r="G52" s="39"/>
+      <c r="H52" s="37"/>
       <c r="I52" s="37"/>
       <c r="J52" s="26"/>
       <c r="K52" s="37"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A53" s="11"/>
-      <c r="B53" s="40"/>
-      <c r="C53" s="40"/>
-      <c r="D53" s="40"/>
-      <c r="E53" s="40"/>
-      <c r="F53" s="40"/>
-      <c r="G53" s="40"/>
-      <c r="H53" s="40"/>
+      <c r="B53" s="39"/>
+      <c r="C53" s="39"/>
+      <c r="D53" s="39"/>
+      <c r="E53" s="39"/>
+      <c r="F53" s="39"/>
+      <c r="G53" s="39"/>
+      <c r="H53" s="37"/>
       <c r="I53" s="37"/>
       <c r="J53" s="26"/>
       <c r="K53" s="37"/>
@@ -1859,13 +1848,13 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A54" s="11"/>
-      <c r="B54" s="40"/>
-      <c r="C54" s="40"/>
-      <c r="D54" s="40"/>
-      <c r="E54" s="40"/>
-      <c r="F54" s="40"/>
-      <c r="G54" s="40"/>
-      <c r="H54" s="40"/>
+      <c r="B54" s="39"/>
+      <c r="C54" s="39"/>
+      <c r="D54" s="39"/>
+      <c r="E54" s="39"/>
+      <c r="F54" s="39"/>
+      <c r="G54" s="39"/>
+      <c r="H54" s="37"/>
       <c r="I54" s="37"/>
       <c r="J54" s="26"/>
       <c r="K54" s="37"/>
@@ -1873,26 +1862,26 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A55" s="11"/>
-      <c r="B55" s="40"/>
-      <c r="C55" s="40"/>
-      <c r="D55" s="40"/>
-      <c r="E55" s="40"/>
-      <c r="F55" s="40"/>
-      <c r="G55" s="40"/>
-      <c r="H55" s="40"/>
+      <c r="B55" s="39"/>
+      <c r="C55" s="39"/>
+      <c r="D55" s="39"/>
+      <c r="E55" s="39"/>
+      <c r="F55" s="39"/>
+      <c r="G55" s="39"/>
+      <c r="H55" s="37"/>
       <c r="I55" s="37"/>
       <c r="K55" s="37"/>
       <c r="M55" s="6"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A56" s="11"/>
-      <c r="B56" s="40"/>
-      <c r="C56" s="40"/>
-      <c r="D56" s="40"/>
-      <c r="E56" s="40"/>
-      <c r="F56" s="40"/>
-      <c r="G56" s="40"/>
-      <c r="H56" s="40"/>
+      <c r="B56" s="39"/>
+      <c r="C56" s="39"/>
+      <c r="D56" s="39"/>
+      <c r="E56" s="39"/>
+      <c r="F56" s="39"/>
+      <c r="G56" s="39"/>
+      <c r="H56" s="37"/>
       <c r="I56" s="37"/>
       <c r="J56" s="7"/>
       <c r="K56" s="37"/>
@@ -1980,13 +1969,13 @@
       <c r="I62" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="J62" s="57">
+      <c r="J62" s="48">
         <f>B5</f>
         <v>0</v>
       </c>
-      <c r="K62" s="57"/>
-      <c r="L62" s="57"/>
-      <c r="M62" s="57"/>
+      <c r="K62" s="48"/>
+      <c r="L62" s="48"/>
+      <c r="M62" s="48"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A63" s="11"/>
@@ -2007,27 +1996,27 @@
       <c r="A64" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B64" s="44" t="s">
+      <c r="B64" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="C64" s="42"/>
-      <c r="D64" s="42"/>
-      <c r="E64" s="42"/>
+      <c r="C64" s="41"/>
+      <c r="D64" s="41"/>
+      <c r="E64" s="41"/>
       <c r="F64" s="25"/>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A65" s="11"/>
-      <c r="B65" s="42" t="s">
+      <c r="B65" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="C65" s="42"/>
-      <c r="D65" s="42"/>
-      <c r="E65" s="42"/>
+      <c r="C65" s="41"/>
+      <c r="D65" s="41"/>
+      <c r="E65" s="41"/>
       <c r="F65" s="25"/>
-      <c r="G65" s="42" t="s">
+      <c r="G65" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="H65" s="42"/>
+      <c r="H65" s="41"/>
       <c r="I65" s="35"/>
       <c r="K65" s="35"/>
       <c r="M65" s="35">
@@ -2042,8 +2031,8 @@
       <c r="D66" s="25"/>
       <c r="E66" s="25"/>
       <c r="F66" s="25"/>
-      <c r="G66" s="42"/>
-      <c r="H66" s="42"/>
+      <c r="G66" s="41"/>
+      <c r="H66" s="41"/>
       <c r="I66" s="22"/>
       <c r="K66" s="22"/>
     </row>
@@ -2077,93 +2066,93 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A69" s="11"/>
-      <c r="B69" s="58" t="s">
+      <c r="B69" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="C69" s="58"/>
-      <c r="D69" s="58"/>
-      <c r="E69" s="58"/>
-      <c r="F69" s="58"/>
-      <c r="G69" s="58"/>
-      <c r="H69" s="58"/>
+      <c r="C69" s="46"/>
+      <c r="D69" s="46"/>
+      <c r="E69" s="46"/>
+      <c r="F69" s="46"/>
+      <c r="G69" s="46"/>
+      <c r="H69" s="46"/>
       <c r="I69" s="7"/>
       <c r="K69" s="7"/>
     </row>
     <row r="70" spans="1:13" ht="15" x14ac:dyDescent="0.15">
       <c r="A70" s="11"/>
-      <c r="B70" s="42" t="s">
+      <c r="B70" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="C70" s="42"/>
-      <c r="D70" s="42"/>
-      <c r="E70" s="42"/>
+      <c r="C70" s="41"/>
+      <c r="D70" s="41"/>
+      <c r="E70" s="41"/>
       <c r="F70" s="25"/>
-      <c r="G70" s="42" t="s">
+      <c r="G70" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="H70" s="42"/>
+      <c r="H70" s="41"/>
       <c r="I70" s="35"/>
       <c r="K70" s="35"/>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A71" s="11"/>
-      <c r="B71" s="42" t="s">
+      <c r="B71" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="C71" s="42"/>
-      <c r="D71" s="42"/>
-      <c r="E71" s="42"/>
+      <c r="C71" s="41"/>
+      <c r="D71" s="41"/>
+      <c r="E71" s="41"/>
       <c r="F71" s="25"/>
-      <c r="G71" s="42" t="s">
+      <c r="G71" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="H71" s="42"/>
+      <c r="H71" s="41"/>
       <c r="I71" s="23"/>
       <c r="K71" s="23"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A72" s="3"/>
-      <c r="B72" s="58" t="s">
+      <c r="B72" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="C72" s="58"/>
-      <c r="D72" s="58"/>
-      <c r="E72" s="58"/>
-      <c r="F72" s="58"/>
-      <c r="G72" s="58"/>
-      <c r="H72" s="58"/>
+      <c r="C72" s="46"/>
+      <c r="D72" s="46"/>
+      <c r="E72" s="46"/>
+      <c r="F72" s="46"/>
+      <c r="G72" s="46"/>
+      <c r="H72" s="46"/>
       <c r="I72" s="7"/>
       <c r="K72" s="7"/>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A73" s="11"/>
-      <c r="B73" s="42" t="s">
+      <c r="B73" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="C73" s="42"/>
-      <c r="D73" s="42"/>
-      <c r="E73" s="42"/>
+      <c r="C73" s="41"/>
+      <c r="D73" s="41"/>
+      <c r="E73" s="41"/>
       <c r="F73" s="25"/>
-      <c r="G73" s="42" t="s">
+      <c r="G73" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="H73" s="42"/>
+      <c r="H73" s="41"/>
       <c r="I73" s="35"/>
       <c r="K73" s="35"/>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A74" s="11"/>
-      <c r="B74" s="42" t="s">
+      <c r="B74" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C74" s="42"/>
-      <c r="D74" s="42"/>
-      <c r="E74" s="42"/>
+      <c r="C74" s="41"/>
+      <c r="D74" s="41"/>
+      <c r="E74" s="41"/>
       <c r="F74" s="25"/>
-      <c r="G74" s="42" t="s">
+      <c r="G74" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="H74" s="42"/>
+      <c r="H74" s="41"/>
       <c r="I74" s="23"/>
       <c r="K74" s="23"/>
     </row>
@@ -2184,34 +2173,34 @@
     </row>
     <row r="76" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="11"/>
-      <c r="B76" s="51" t="s">
+      <c r="B76" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="C76" s="51"/>
-      <c r="D76" s="51"/>
-      <c r="E76" s="51"/>
-      <c r="F76" s="51"/>
-      <c r="G76" s="51" t="s">
+      <c r="C76" s="42"/>
+      <c r="D76" s="42"/>
+      <c r="E76" s="42"/>
+      <c r="F76" s="42"/>
+      <c r="G76" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="H76" s="51"/>
+      <c r="H76" s="42"/>
       <c r="I76" s="35"/>
       <c r="J76" s="1"/>
       <c r="K76" s="35"/>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A77" s="11"/>
-      <c r="B77" s="42" t="s">
+      <c r="B77" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="C77" s="42"/>
-      <c r="D77" s="42"/>
-      <c r="E77" s="42"/>
+      <c r="C77" s="41"/>
+      <c r="D77" s="41"/>
+      <c r="E77" s="41"/>
       <c r="F77" s="25"/>
-      <c r="G77" s="42" t="s">
+      <c r="G77" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="H77" s="42"/>
+      <c r="H77" s="41"/>
       <c r="I77" s="35"/>
       <c r="J77" s="1"/>
       <c r="K77" s="35"/>
@@ -2224,59 +2213,59 @@
       <c r="D78" s="30"/>
       <c r="E78" s="30"/>
       <c r="F78" s="30"/>
-      <c r="G78" s="51" t="s">
+      <c r="G78" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="H78" s="51"/>
+      <c r="H78" s="42"/>
       <c r="I78" s="35"/>
       <c r="J78" s="1"/>
       <c r="K78" s="35"/>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A79" s="11"/>
-      <c r="B79" s="42" t="s">
+      <c r="B79" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="C79" s="42"/>
-      <c r="D79" s="42"/>
-      <c r="E79" s="42"/>
+      <c r="C79" s="41"/>
+      <c r="D79" s="41"/>
+      <c r="E79" s="41"/>
       <c r="F79" s="25"/>
-      <c r="G79" s="42" t="s">
+      <c r="G79" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="H79" s="42"/>
+      <c r="H79" s="41"/>
       <c r="I79" s="35"/>
       <c r="K79" s="35"/>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A80" s="11"/>
-      <c r="B80" s="42" t="s">
+      <c r="B80" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="C80" s="42"/>
-      <c r="D80" s="42"/>
-      <c r="E80" s="42"/>
+      <c r="C80" s="41"/>
+      <c r="D80" s="41"/>
+      <c r="E80" s="41"/>
       <c r="F80" s="25"/>
-      <c r="G80" s="42" t="s">
+      <c r="G80" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="H80" s="42"/>
+      <c r="H80" s="41"/>
       <c r="I80" s="6"/>
       <c r="K80" s="6"/>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A81" s="11"/>
-      <c r="B81" s="42" t="s">
+      <c r="B81" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="C81" s="42"/>
-      <c r="D81" s="42"/>
-      <c r="E81" s="42"/>
+      <c r="C81" s="41"/>
+      <c r="D81" s="41"/>
+      <c r="E81" s="41"/>
       <c r="F81" s="25"/>
-      <c r="G81" s="42" t="s">
+      <c r="G81" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="H81" s="42"/>
+      <c r="H81" s="41"/>
       <c r="I81" s="23"/>
       <c r="K81" s="23"/>
     </row>
@@ -2293,27 +2282,27 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A83" s="11"/>
-      <c r="B83" s="42" t="s">
+      <c r="B83" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="C83" s="42"/>
-      <c r="D83" s="42"/>
-      <c r="E83" s="42"/>
-      <c r="F83" s="42"/>
-      <c r="G83" s="42"/>
-      <c r="H83" s="42"/>
-      <c r="I83" s="42"/>
-      <c r="J83" s="42"/>
-      <c r="K83" s="42"/>
+      <c r="C83" s="41"/>
+      <c r="D83" s="41"/>
+      <c r="E83" s="41"/>
+      <c r="F83" s="41"/>
+      <c r="G83" s="41"/>
+      <c r="H83" s="41"/>
+      <c r="I83" s="41"/>
+      <c r="J83" s="41"/>
+      <c r="K83" s="41"/>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A84" s="11"/>
-      <c r="B84" s="42" t="s">
+      <c r="B84" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="C84" s="42"/>
-      <c r="D84" s="42"/>
-      <c r="E84" s="42"/>
+      <c r="C84" s="41"/>
+      <c r="D84" s="41"/>
+      <c r="E84" s="41"/>
       <c r="F84" s="25"/>
       <c r="G84" s="25"/>
       <c r="H84" s="25"/>
@@ -2323,12 +2312,12 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A85" s="11"/>
-      <c r="B85" s="42" t="s">
+      <c r="B85" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="C85" s="42"/>
-      <c r="D85" s="42"/>
-      <c r="E85" s="42"/>
+      <c r="C85" s="41"/>
+      <c r="D85" s="41"/>
+      <c r="E85" s="41"/>
       <c r="F85" s="25"/>
       <c r="G85" s="25"/>
       <c r="H85" s="25"/>
@@ -2337,12 +2326,12 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A86" s="11"/>
-      <c r="B86" s="42" t="s">
+      <c r="B86" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="C86" s="42"/>
-      <c r="D86" s="42"/>
-      <c r="E86" s="42"/>
+      <c r="C86" s="41"/>
+      <c r="D86" s="41"/>
+      <c r="E86" s="41"/>
       <c r="F86" s="25"/>
       <c r="G86" s="25"/>
       <c r="H86" s="25"/>
@@ -2351,12 +2340,12 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A87" s="11"/>
-      <c r="B87" s="42" t="s">
+      <c r="B87" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="C87" s="42"/>
-      <c r="D87" s="42"/>
-      <c r="E87" s="42"/>
+      <c r="C87" s="41"/>
+      <c r="D87" s="41"/>
+      <c r="E87" s="41"/>
       <c r="F87" s="25"/>
       <c r="G87" s="25"/>
       <c r="H87" s="25"/>
@@ -2365,12 +2354,12 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A88" s="11"/>
-      <c r="B88" s="42" t="s">
+      <c r="B88" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="C88" s="42"/>
-      <c r="D88" s="42"/>
-      <c r="E88" s="42"/>
+      <c r="C88" s="41"/>
+      <c r="D88" s="41"/>
+      <c r="E88" s="41"/>
       <c r="F88" s="25"/>
       <c r="G88" s="25"/>
       <c r="H88" s="25"/>
@@ -2412,12 +2401,12 @@
       <c r="A92" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B92" s="44" t="s">
+      <c r="B92" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="C92" s="42"/>
-      <c r="D92" s="42"/>
-      <c r="E92" s="42"/>
+      <c r="C92" s="41"/>
+      <c r="D92" s="41"/>
+      <c r="E92" s="41"/>
       <c r="F92" s="25"/>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.15">
@@ -2475,16 +2464,16 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A97" s="11"/>
-      <c r="B97" s="42"/>
-      <c r="C97" s="42"/>
-      <c r="D97" s="42"/>
-      <c r="E97" s="42"/>
-      <c r="F97" s="42"/>
-      <c r="G97" s="42"/>
-      <c r="H97" s="42"/>
-      <c r="I97" s="42"/>
-      <c r="J97" s="42"/>
-      <c r="K97" s="42"/>
+      <c r="B97" s="41"/>
+      <c r="C97" s="41"/>
+      <c r="D97" s="41"/>
+      <c r="E97" s="41"/>
+      <c r="F97" s="41"/>
+      <c r="G97" s="41"/>
+      <c r="H97" s="41"/>
+      <c r="I97" s="41"/>
+      <c r="J97" s="41"/>
+      <c r="K97" s="41"/>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A98" s="11"/>
@@ -2503,47 +2492,47 @@
       <c r="A99" s="11"/>
       <c r="J99" s="29"/>
       <c r="K99" s="33"/>
-      <c r="L99" s="50" t="s">
+      <c r="L99" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="M99" s="50"/>
+      <c r="M99" s="47"/>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A100" s="11"/>
       <c r="B100" s="35"/>
-      <c r="C100" s="42" t="s">
+      <c r="C100" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="D100" s="42"/>
-      <c r="E100" s="42"/>
-      <c r="F100" s="42"/>
-      <c r="G100" s="42"/>
+      <c r="D100" s="41"/>
+      <c r="E100" s="41"/>
+      <c r="F100" s="41"/>
+      <c r="G100" s="41"/>
       <c r="H100" s="37"/>
       <c r="I100" s="36"/>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A101" s="11"/>
       <c r="B101" s="23"/>
-      <c r="C101" s="42" t="s">
+      <c r="C101" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="D101" s="42"/>
-      <c r="E101" s="42"/>
-      <c r="F101" s="42"/>
-      <c r="G101" s="42"/>
+      <c r="D101" s="41"/>
+      <c r="E101" s="41"/>
+      <c r="F101" s="41"/>
+      <c r="G101" s="41"/>
       <c r="H101" s="37"/>
       <c r="I101" s="36"/>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A102" s="11"/>
       <c r="B102" s="22"/>
-      <c r="C102" s="42"/>
-      <c r="D102" s="42"/>
-      <c r="E102" s="42"/>
-      <c r="F102" s="42"/>
-      <c r="G102" s="42"/>
-      <c r="H102" s="59"/>
-      <c r="I102" s="59"/>
+      <c r="C102" s="41"/>
+      <c r="D102" s="41"/>
+      <c r="E102" s="41"/>
+      <c r="F102" s="41"/>
+      <c r="G102" s="41"/>
+      <c r="H102" s="44"/>
+      <c r="I102" s="44"/>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A103" s="11"/>
@@ -2585,9 +2574,9 @@
       <c r="A106" s="11"/>
       <c r="B106" s="1"/>
     </row>
-    <row r="107" spans="1:13" ht="15" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A107" s="11"/>
-      <c r="B107" s="39" t="s">
+      <c r="B107" s="3" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2622,21 +2611,54 @@
     </row>
   </sheetData>
   <mergeCells count="83">
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="B46:H46"/>
-    <mergeCell ref="G74:H74"/>
-    <mergeCell ref="G78:H78"/>
-    <mergeCell ref="B77:E77"/>
-    <mergeCell ref="G77:H77"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="C104:F104"/>
-    <mergeCell ref="G79:H79"/>
-    <mergeCell ref="C102:G102"/>
-    <mergeCell ref="C100:G100"/>
-    <mergeCell ref="H102:I102"/>
-    <mergeCell ref="G81:H81"/>
-    <mergeCell ref="B88:E88"/>
-    <mergeCell ref="B83:K83"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="L99:M99"/>
+    <mergeCell ref="B97:K97"/>
+    <mergeCell ref="J62:M62"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="B81:E81"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="B70:E70"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B42:H42"/>
     <mergeCell ref="B38:M38"/>
     <mergeCell ref="C101:G101"/>
     <mergeCell ref="B71:E71"/>
@@ -2653,58 +2675,25 @@
     <mergeCell ref="B43:H43"/>
     <mergeCell ref="B44:H44"/>
     <mergeCell ref="B72:H72"/>
+    <mergeCell ref="C104:F104"/>
+    <mergeCell ref="G79:H79"/>
+    <mergeCell ref="C102:G102"/>
+    <mergeCell ref="C100:G100"/>
+    <mergeCell ref="H102:I102"/>
+    <mergeCell ref="G81:H81"/>
+    <mergeCell ref="B88:E88"/>
+    <mergeCell ref="B83:K83"/>
     <mergeCell ref="B84:E84"/>
     <mergeCell ref="B85:E85"/>
     <mergeCell ref="B86:E86"/>
     <mergeCell ref="B92:E92"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="L99:M99"/>
-    <mergeCell ref="B97:K97"/>
-    <mergeCell ref="J62:M62"/>
-    <mergeCell ref="G73:H73"/>
-    <mergeCell ref="B81:E81"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="B70:E70"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="B76:F76"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="B1:M1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="G74:H74"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="B77:E77"/>
+    <mergeCell ref="G77:H77"/>
+    <mergeCell ref="B74:E74"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update readme and other small fixes
</commit_message>
<xml_diff>
--- a/blankPPF.xlsx
+++ b/blankPPF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshpopp/Downloads/ppfproj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF89016-B7BA-AF49-95BB-5226D298993E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1E6912-1FFD-874B-9FF1-EAD66EFF89FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6660" yWindow="920" windowWidth="19500" windowHeight="14360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6100" yWindow="920" windowWidth="19500" windowHeight="14360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PPF 2007" sheetId="1" r:id="rId1"/>
@@ -447,9 +447,6 @@
     <t>ENGRI 1xxx</t>
   </si>
   <si>
-    <t>BEE 1200</t>
-  </si>
-  <si>
     <t>(Minimum 128)</t>
   </si>
   <si>
@@ -489,6 +486,9 @@
   <si>
     <t>a) Engineering distribution requirement is satisfied by ENGRD 2020 and ENGRD 2600 or ENGRD 2510</t>
   </si>
+  <si>
+    <t>BEE 1200/ ENGRG 1050</t>
+  </si>
 </sst>
 </file>
 
@@ -497,7 +497,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/yyyy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -521,6 +521,12 @@
     </font>
     <font>
       <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -593,7 +599,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -671,22 +677,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -694,6 +694,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -708,10 +714,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1053,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K31" activeCellId="1" sqref="I31 K31"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I104" sqref="I104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1075,54 +1087,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
       <c r="N1" s="12"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
       <c r="N2" s="2"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="B3" s="57" t="s">
-        <v>107</v>
-      </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
+      <c r="B3" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
       <c r="N3" s="2"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.15">
@@ -1130,21 +1142,21 @@
         <v>11</v>
       </c>
       <c r="B5" s="43"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
       <c r="F5" s="26"/>
       <c r="G5" s="26"/>
       <c r="I5" s="25"/>
-      <c r="J5" s="45" t="s">
+      <c r="J5" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="45"/>
-      <c r="L5" s="58">
+      <c r="K5" s="44"/>
+      <c r="L5" s="46">
         <f ca="1">TODAY()</f>
         <v>43816</v>
       </c>
-      <c r="M5" s="58"/>
+      <c r="M5" s="46"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6" s="34" t="s">
@@ -1152,20 +1164,20 @@
       </c>
       <c r="B6" s="43"/>
       <c r="C6" s="43"/>
-      <c r="D6" s="51" t="s">
+      <c r="D6" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="45" t="s">
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="45"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="42"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7" s="24" t="s">
@@ -1174,15 +1186,15 @@
       <c r="B7" s="43"/>
       <c r="C7" s="43"/>
       <c r="D7" s="43"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
       <c r="I7" s="25"/>
-      <c r="J7" s="45" t="s">
+      <c r="J7" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="44"/>
       <c r="M7" s="14"/>
     </row>
     <row r="8" spans="1:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
@@ -1247,12 +1259,12 @@
       <c r="A11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
       <c r="F11" s="26"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.15">
@@ -1261,8 +1273,8 @@
         <v>16</v>
       </c>
       <c r="C12" s="43"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
       <c r="F12" s="25"/>
       <c r="G12" s="43" t="s">
         <v>94</v>
@@ -1274,11 +1286,11 @@
     <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13" s="11"/>
       <c r="B13" s="43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C13" s="43"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
       <c r="F13" s="25"/>
       <c r="G13" s="43" t="s">
         <v>95</v>
@@ -1293,8 +1305,8 @@
         <v>38</v>
       </c>
       <c r="C14" s="43"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
       <c r="F14" s="25"/>
       <c r="G14" s="43" t="s">
         <v>51</v>
@@ -1309,8 +1321,8 @@
         <v>39</v>
       </c>
       <c r="C15" s="43"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
       <c r="F15" s="25"/>
       <c r="G15" s="43" t="s">
         <v>52</v>
@@ -1325,13 +1337,13 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A16" s="11"/>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A17" s="11"/>
@@ -1340,43 +1352,43 @@
       <c r="A18" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
       <c r="F18" s="25"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A19" s="11"/>
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="41" t="s">
+      <c r="G19" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="H19" s="41"/>
+      <c r="H19" s="42"/>
       <c r="I19" s="35"/>
       <c r="K19" s="35"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A20" s="11"/>
-      <c r="B20" s="41" t="s">
+      <c r="B20" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
       <c r="F20" s="25"/>
-      <c r="G20" s="41" t="s">
+      <c r="G20" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="41"/>
+      <c r="H20" s="42"/>
       <c r="I20" s="35"/>
       <c r="K20" s="23"/>
       <c r="M20" s="35">
@@ -1392,12 +1404,12 @@
       <c r="A22" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="45" t="s">
+      <c r="B22" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
       <c r="F22" s="25"/>
       <c r="I22" s="6"/>
       <c r="J22" s="7"/>
@@ -1407,29 +1419,29 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A23" s="11"/>
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
       <c r="F23" s="25"/>
-      <c r="G23" s="41" t="s">
+      <c r="G23" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="H23" s="41"/>
+      <c r="H23" s="42"/>
       <c r="I23" s="35"/>
       <c r="K23" s="35"/>
       <c r="M23" s="6"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A24" s="11"/>
-      <c r="B24" s="41" t="s">
+      <c r="B24" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
       <c r="G24" s="25" t="s">
         <v>60</v>
       </c>
@@ -1530,7 +1542,7 @@
     <row r="32" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A32" s="11"/>
       <c r="B32" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C32" s="25"/>
       <c r="D32" s="25"/>
@@ -1564,7 +1576,7 @@
         <v>22</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C34" s="25"/>
       <c r="D34" s="25"/>
@@ -1617,20 +1629,20 @@
       <c r="A38" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="45" t="s">
+      <c r="B38" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="41"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="41"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
-      <c r="J38" s="41"/>
-      <c r="K38" s="41"/>
-      <c r="L38" s="41"/>
-      <c r="M38" s="41"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="42"/>
+      <c r="G38" s="42"/>
+      <c r="H38" s="42"/>
+      <c r="I38" s="42"/>
+      <c r="J38" s="42"/>
+      <c r="K38" s="42"/>
+      <c r="L38" s="42"/>
+      <c r="M38" s="42"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A39" s="11"/>
@@ -1666,29 +1678,29 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A41" s="11"/>
-      <c r="B41" s="42" t="s">
+      <c r="B41" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="C41" s="42"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="42"/>
-      <c r="F41" s="42"/>
-      <c r="G41" s="42"/>
-      <c r="H41" s="42"/>
+      <c r="C41" s="51"/>
+      <c r="D41" s="51"/>
+      <c r="E41" s="51"/>
+      <c r="F41" s="51"/>
+      <c r="G41" s="51"/>
+      <c r="H41" s="51"/>
       <c r="I41" s="6"/>
       <c r="K41" s="6"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A42" s="11"/>
-      <c r="B42" s="42" t="s">
+      <c r="B42" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="42"/>
-      <c r="F42" s="42"/>
-      <c r="G42" s="42"/>
-      <c r="H42" s="42"/>
+      <c r="C42" s="51"/>
+      <c r="D42" s="51"/>
+      <c r="E42" s="51"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="51"/>
+      <c r="H42" s="51"/>
       <c r="I42" s="6"/>
       <c r="J42" s="7"/>
       <c r="K42" s="6"/>
@@ -1696,15 +1708,15 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A43" s="11"/>
-      <c r="B43" s="42" t="s">
+      <c r="B43" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="42"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="42"/>
-      <c r="F43" s="42"/>
-      <c r="G43" s="42"/>
-      <c r="H43" s="42"/>
+      <c r="C43" s="51"/>
+      <c r="D43" s="51"/>
+      <c r="E43" s="51"/>
+      <c r="F43" s="51"/>
+      <c r="G43" s="51"/>
+      <c r="H43" s="51"/>
       <c r="I43" s="7"/>
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
@@ -1712,15 +1724,15 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A44" s="11"/>
-      <c r="B44" s="42" t="s">
+      <c r="B44" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="C44" s="42"/>
-      <c r="D44" s="42"/>
-      <c r="E44" s="42"/>
-      <c r="F44" s="42"/>
-      <c r="G44" s="42"/>
-      <c r="H44" s="42"/>
+      <c r="C44" s="51"/>
+      <c r="D44" s="51"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="51"/>
+      <c r="H44" s="51"/>
       <c r="I44" s="7"/>
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
@@ -1728,15 +1740,15 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A45" s="11"/>
-      <c r="B45" s="42" t="s">
+      <c r="B45" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="42"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="42"/>
-      <c r="F45" s="42"/>
-      <c r="G45" s="42"/>
-      <c r="H45" s="42"/>
+      <c r="C45" s="51"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="51"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="51"/>
+      <c r="H45" s="51"/>
       <c r="I45" s="6"/>
       <c r="J45" s="7"/>
       <c r="K45" s="6"/>
@@ -1744,15 +1756,15 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A46" s="11"/>
-      <c r="B46" s="42" t="s">
+      <c r="B46" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="C46" s="42"/>
-      <c r="D46" s="42"/>
-      <c r="E46" s="42"/>
-      <c r="F46" s="42"/>
-      <c r="G46" s="42"/>
-      <c r="H46" s="42"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="51"/>
+      <c r="F46" s="51"/>
+      <c r="G46" s="51"/>
+      <c r="H46" s="51"/>
       <c r="I46" s="6"/>
       <c r="J46" s="7"/>
       <c r="K46" s="6"/>
@@ -1969,13 +1981,13 @@
       <c r="I62" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="J62" s="48">
+      <c r="J62" s="57">
         <f>B5</f>
         <v>0</v>
       </c>
-      <c r="K62" s="48"/>
-      <c r="L62" s="48"/>
-      <c r="M62" s="48"/>
+      <c r="K62" s="57"/>
+      <c r="L62" s="57"/>
+      <c r="M62" s="57"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A63" s="11"/>
@@ -1996,27 +2008,27 @@
       <c r="A64" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B64" s="45" t="s">
+      <c r="B64" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="C64" s="41"/>
-      <c r="D64" s="41"/>
-      <c r="E64" s="41"/>
+      <c r="C64" s="42"/>
+      <c r="D64" s="42"/>
+      <c r="E64" s="42"/>
       <c r="F64" s="25"/>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A65" s="11"/>
-      <c r="B65" s="41" t="s">
+      <c r="B65" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="C65" s="41"/>
-      <c r="D65" s="41"/>
-      <c r="E65" s="41"/>
+      <c r="C65" s="42"/>
+      <c r="D65" s="42"/>
+      <c r="E65" s="42"/>
       <c r="F65" s="25"/>
-      <c r="G65" s="41" t="s">
+      <c r="G65" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="H65" s="41"/>
+      <c r="H65" s="42"/>
       <c r="I65" s="35"/>
       <c r="K65" s="35"/>
       <c r="M65" s="35">
@@ -2031,8 +2043,8 @@
       <c r="D66" s="25"/>
       <c r="E66" s="25"/>
       <c r="F66" s="25"/>
-      <c r="G66" s="41"/>
-      <c r="H66" s="41"/>
+      <c r="G66" s="42"/>
+      <c r="H66" s="42"/>
       <c r="I66" s="22"/>
       <c r="K66" s="22"/>
     </row>
@@ -2066,93 +2078,93 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A69" s="11"/>
-      <c r="B69" s="46" t="s">
+      <c r="B69" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="C69" s="46"/>
-      <c r="D69" s="46"/>
-      <c r="E69" s="46"/>
-      <c r="F69" s="46"/>
-      <c r="G69" s="46"/>
-      <c r="H69" s="46"/>
+      <c r="C69" s="58"/>
+      <c r="D69" s="58"/>
+      <c r="E69" s="58"/>
+      <c r="F69" s="58"/>
+      <c r="G69" s="58"/>
+      <c r="H69" s="58"/>
       <c r="I69" s="7"/>
       <c r="K69" s="7"/>
     </row>
     <row r="70" spans="1:13" ht="15" x14ac:dyDescent="0.15">
       <c r="A70" s="11"/>
-      <c r="B70" s="41" t="s">
+      <c r="B70" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="C70" s="41"/>
-      <c r="D70" s="41"/>
-      <c r="E70" s="41"/>
+      <c r="C70" s="42"/>
+      <c r="D70" s="42"/>
+      <c r="E70" s="42"/>
       <c r="F70" s="25"/>
-      <c r="G70" s="41" t="s">
+      <c r="G70" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="H70" s="41"/>
+      <c r="H70" s="42"/>
       <c r="I70" s="35"/>
       <c r="K70" s="35"/>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A71" s="11"/>
-      <c r="B71" s="41" t="s">
+      <c r="B71" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="C71" s="41"/>
-      <c r="D71" s="41"/>
-      <c r="E71" s="41"/>
+      <c r="C71" s="42"/>
+      <c r="D71" s="42"/>
+      <c r="E71" s="42"/>
       <c r="F71" s="25"/>
-      <c r="G71" s="41" t="s">
+      <c r="G71" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="H71" s="41"/>
+      <c r="H71" s="42"/>
       <c r="I71" s="23"/>
       <c r="K71" s="23"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A72" s="3"/>
-      <c r="B72" s="46" t="s">
+      <c r="B72" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="C72" s="46"/>
-      <c r="D72" s="46"/>
-      <c r="E72" s="46"/>
-      <c r="F72" s="46"/>
-      <c r="G72" s="46"/>
-      <c r="H72" s="46"/>
+      <c r="C72" s="58"/>
+      <c r="D72" s="58"/>
+      <c r="E72" s="58"/>
+      <c r="F72" s="58"/>
+      <c r="G72" s="58"/>
+      <c r="H72" s="58"/>
       <c r="I72" s="7"/>
       <c r="K72" s="7"/>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A73" s="11"/>
-      <c r="B73" s="41" t="s">
+      <c r="B73" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="C73" s="41"/>
-      <c r="D73" s="41"/>
-      <c r="E73" s="41"/>
+      <c r="C73" s="42"/>
+      <c r="D73" s="42"/>
+      <c r="E73" s="42"/>
       <c r="F73" s="25"/>
-      <c r="G73" s="41" t="s">
+      <c r="G73" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="H73" s="41"/>
+      <c r="H73" s="42"/>
       <c r="I73" s="35"/>
       <c r="K73" s="35"/>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A74" s="11"/>
-      <c r="B74" s="41" t="s">
+      <c r="B74" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C74" s="41"/>
-      <c r="D74" s="41"/>
-      <c r="E74" s="41"/>
+      <c r="C74" s="42"/>
+      <c r="D74" s="42"/>
+      <c r="E74" s="42"/>
       <c r="F74" s="25"/>
-      <c r="G74" s="41" t="s">
+      <c r="G74" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="H74" s="41"/>
+      <c r="H74" s="42"/>
       <c r="I74" s="23"/>
       <c r="K74" s="23"/>
     </row>
@@ -2164,7 +2176,7 @@
       <c r="E75" s="25"/>
       <c r="F75" s="25"/>
       <c r="G75" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H75" s="25"/>
       <c r="I75" s="6"/>
@@ -2173,34 +2185,34 @@
     </row>
     <row r="76" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="11"/>
-      <c r="B76" s="42" t="s">
+      <c r="B76" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="C76" s="42"/>
-      <c r="D76" s="42"/>
-      <c r="E76" s="42"/>
-      <c r="F76" s="42"/>
-      <c r="G76" s="42" t="s">
+      <c r="C76" s="51"/>
+      <c r="D76" s="51"/>
+      <c r="E76" s="51"/>
+      <c r="F76" s="51"/>
+      <c r="G76" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="H76" s="42"/>
+      <c r="H76" s="51"/>
       <c r="I76" s="35"/>
       <c r="J76" s="1"/>
       <c r="K76" s="35"/>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A77" s="11"/>
-      <c r="B77" s="41" t="s">
+      <c r="B77" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="C77" s="41"/>
-      <c r="D77" s="41"/>
-      <c r="E77" s="41"/>
+      <c r="C77" s="42"/>
+      <c r="D77" s="42"/>
+      <c r="E77" s="42"/>
       <c r="F77" s="25"/>
-      <c r="G77" s="41" t="s">
+      <c r="G77" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="H77" s="41"/>
+      <c r="H77" s="42"/>
       <c r="I77" s="35"/>
       <c r="J77" s="1"/>
       <c r="K77" s="35"/>
@@ -2213,59 +2225,59 @@
       <c r="D78" s="30"/>
       <c r="E78" s="30"/>
       <c r="F78" s="30"/>
-      <c r="G78" s="42" t="s">
+      <c r="G78" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="H78" s="42"/>
+      <c r="H78" s="51"/>
       <c r="I78" s="35"/>
       <c r="J78" s="1"/>
       <c r="K78" s="35"/>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A79" s="11"/>
-      <c r="B79" s="41" t="s">
+      <c r="B79" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="C79" s="41"/>
-      <c r="D79" s="41"/>
-      <c r="E79" s="41"/>
+      <c r="C79" s="42"/>
+      <c r="D79" s="42"/>
+      <c r="E79" s="42"/>
       <c r="F79" s="25"/>
-      <c r="G79" s="41" t="s">
+      <c r="G79" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="H79" s="41"/>
+      <c r="H79" s="42"/>
       <c r="I79" s="35"/>
       <c r="K79" s="35"/>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A80" s="11"/>
-      <c r="B80" s="41" t="s">
+      <c r="B80" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="C80" s="41"/>
-      <c r="D80" s="41"/>
-      <c r="E80" s="41"/>
+      <c r="C80" s="42"/>
+      <c r="D80" s="42"/>
+      <c r="E80" s="42"/>
       <c r="F80" s="25"/>
-      <c r="G80" s="41" t="s">
+      <c r="G80" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="H80" s="41"/>
+      <c r="H80" s="42"/>
       <c r="I80" s="6"/>
       <c r="K80" s="6"/>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A81" s="11"/>
-      <c r="B81" s="41" t="s">
+      <c r="B81" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="C81" s="41"/>
-      <c r="D81" s="41"/>
-      <c r="E81" s="41"/>
+      <c r="C81" s="42"/>
+      <c r="D81" s="42"/>
+      <c r="E81" s="42"/>
       <c r="F81" s="25"/>
-      <c r="G81" s="41" t="s">
+      <c r="G81" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="H81" s="41"/>
+      <c r="H81" s="42"/>
       <c r="I81" s="23"/>
       <c r="K81" s="23"/>
     </row>
@@ -2282,27 +2294,27 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A83" s="11"/>
-      <c r="B83" s="41" t="s">
-        <v>106</v>
-      </c>
-      <c r="C83" s="41"/>
-      <c r="D83" s="41"/>
-      <c r="E83" s="41"/>
-      <c r="F83" s="41"/>
-      <c r="G83" s="41"/>
-      <c r="H83" s="41"/>
-      <c r="I83" s="41"/>
-      <c r="J83" s="41"/>
-      <c r="K83" s="41"/>
+      <c r="B83" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="C83" s="42"/>
+      <c r="D83" s="42"/>
+      <c r="E83" s="42"/>
+      <c r="F83" s="42"/>
+      <c r="G83" s="42"/>
+      <c r="H83" s="42"/>
+      <c r="I83" s="42"/>
+      <c r="J83" s="42"/>
+      <c r="K83" s="42"/>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A84" s="11"/>
-      <c r="B84" s="41" t="s">
+      <c r="B84" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="C84" s="41"/>
-      <c r="D84" s="41"/>
-      <c r="E84" s="41"/>
+      <c r="C84" s="42"/>
+      <c r="D84" s="42"/>
+      <c r="E84" s="42"/>
       <c r="F84" s="25"/>
       <c r="G84" s="25"/>
       <c r="H84" s="25"/>
@@ -2312,12 +2324,12 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A85" s="11"/>
-      <c r="B85" s="41" t="s">
+      <c r="B85" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="C85" s="41"/>
-      <c r="D85" s="41"/>
-      <c r="E85" s="41"/>
+      <c r="C85" s="42"/>
+      <c r="D85" s="42"/>
+      <c r="E85" s="42"/>
       <c r="F85" s="25"/>
       <c r="G85" s="25"/>
       <c r="H85" s="25"/>
@@ -2326,12 +2338,12 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A86" s="11"/>
-      <c r="B86" s="41" t="s">
+      <c r="B86" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="C86" s="41"/>
-      <c r="D86" s="41"/>
-      <c r="E86" s="41"/>
+      <c r="C86" s="42"/>
+      <c r="D86" s="42"/>
+      <c r="E86" s="42"/>
       <c r="F86" s="25"/>
       <c r="G86" s="25"/>
       <c r="H86" s="25"/>
@@ -2340,12 +2352,12 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A87" s="11"/>
-      <c r="B87" s="41" t="s">
+      <c r="B87" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="C87" s="41"/>
-      <c r="D87" s="41"/>
-      <c r="E87" s="41"/>
+      <c r="C87" s="42"/>
+      <c r="D87" s="42"/>
+      <c r="E87" s="42"/>
       <c r="F87" s="25"/>
       <c r="G87" s="25"/>
       <c r="H87" s="25"/>
@@ -2354,12 +2366,12 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A88" s="11"/>
-      <c r="B88" s="41" t="s">
+      <c r="B88" s="42" t="s">
         <v>88</v>
       </c>
-      <c r="C88" s="41"/>
-      <c r="D88" s="41"/>
-      <c r="E88" s="41"/>
+      <c r="C88" s="42"/>
+      <c r="D88" s="42"/>
+      <c r="E88" s="42"/>
       <c r="F88" s="25"/>
       <c r="G88" s="25"/>
       <c r="H88" s="25"/>
@@ -2401,13 +2413,16 @@
       <c r="A92" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B92" s="45" t="s">
+      <c r="B92" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="C92" s="41"/>
-      <c r="D92" s="41"/>
-      <c r="E92" s="41"/>
+      <c r="C92" s="42"/>
+      <c r="D92" s="42"/>
+      <c r="E92" s="42"/>
       <c r="F92" s="25"/>
+      <c r="I92" s="41"/>
+      <c r="J92" s="7"/>
+      <c r="K92" s="41"/>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A93" s="11"/>
@@ -2444,10 +2459,6 @@
       <c r="H95" s="25"/>
       <c r="I95" s="23"/>
       <c r="K95" s="23"/>
-      <c r="M95" s="35">
-        <f>SUM(K93:K95)</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A96" s="11"/>
@@ -2458,22 +2469,25 @@
       <c r="F96" s="25"/>
       <c r="G96" s="25"/>
       <c r="H96" s="25"/>
-      <c r="I96" s="6"/>
-      <c r="K96" s="6"/>
-      <c r="M96" s="6"/>
+      <c r="I96" s="60"/>
+      <c r="K96" s="60"/>
+      <c r="M96" s="35">
+        <f>SUM(K93:K95)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A97" s="11"/>
-      <c r="B97" s="41"/>
-      <c r="C97" s="41"/>
-      <c r="D97" s="41"/>
-      <c r="E97" s="41"/>
-      <c r="F97" s="41"/>
-      <c r="G97" s="41"/>
-      <c r="H97" s="41"/>
-      <c r="I97" s="41"/>
-      <c r="J97" s="41"/>
-      <c r="K97" s="41"/>
+      <c r="B97" s="42"/>
+      <c r="C97" s="42"/>
+      <c r="D97" s="42"/>
+      <c r="E97" s="42"/>
+      <c r="F97" s="42"/>
+      <c r="G97" s="42"/>
+      <c r="H97" s="42"/>
+      <c r="I97" s="42"/>
+      <c r="J97" s="42"/>
+      <c r="K97" s="42"/>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A98" s="11"/>
@@ -2484,7 +2498,7 @@
       <c r="K98" s="1"/>
       <c r="L98" s="1"/>
       <c r="M98" s="35">
-        <f>SUM(M15:M95)</f>
+        <f>SUM(M15:M96)</f>
         <v>0</v>
       </c>
     </row>
@@ -2492,47 +2506,47 @@
       <c r="A99" s="11"/>
       <c r="J99" s="29"/>
       <c r="K99" s="33"/>
-      <c r="L99" s="47" t="s">
-        <v>105</v>
-      </c>
-      <c r="M99" s="47"/>
+      <c r="L99" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="M99" s="50"/>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A100" s="11"/>
       <c r="B100" s="35"/>
-      <c r="C100" s="41" t="s">
+      <c r="C100" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="D100" s="41"/>
-      <c r="E100" s="41"/>
-      <c r="F100" s="41"/>
-      <c r="G100" s="41"/>
+      <c r="D100" s="42"/>
+      <c r="E100" s="42"/>
+      <c r="F100" s="42"/>
+      <c r="G100" s="42"/>
       <c r="H100" s="37"/>
       <c r="I100" s="36"/>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A101" s="11"/>
       <c r="B101" s="23"/>
-      <c r="C101" s="41" t="s">
+      <c r="C101" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="D101" s="41"/>
-      <c r="E101" s="41"/>
-      <c r="F101" s="41"/>
-      <c r="G101" s="41"/>
+      <c r="D101" s="42"/>
+      <c r="E101" s="42"/>
+      <c r="F101" s="42"/>
+      <c r="G101" s="42"/>
       <c r="H101" s="37"/>
       <c r="I101" s="36"/>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A102" s="11"/>
       <c r="B102" s="22"/>
-      <c r="C102" s="41"/>
-      <c r="D102" s="41"/>
-      <c r="E102" s="41"/>
-      <c r="F102" s="41"/>
-      <c r="G102" s="41"/>
-      <c r="H102" s="44"/>
-      <c r="I102" s="44"/>
+      <c r="C102" s="42"/>
+      <c r="D102" s="42"/>
+      <c r="E102" s="42"/>
+      <c r="F102" s="42"/>
+      <c r="G102" s="42"/>
+      <c r="H102" s="59"/>
+      <c r="I102" s="59"/>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A103" s="11"/>
@@ -2556,7 +2570,7 @@
       <c r="F104" s="43"/>
       <c r="G104" s="21"/>
       <c r="H104" s="3" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.15">
@@ -2577,7 +2591,7 @@
     <row r="107" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A107" s="11"/>
       <c r="B107" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.15">
@@ -2611,6 +2625,73 @@
     </row>
   </sheetData>
   <mergeCells count="83">
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="G74:H74"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="B77:E77"/>
+    <mergeCell ref="G77:H77"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="C104:F104"/>
+    <mergeCell ref="G79:H79"/>
+    <mergeCell ref="C102:G102"/>
+    <mergeCell ref="C100:G100"/>
+    <mergeCell ref="H102:I102"/>
+    <mergeCell ref="G81:H81"/>
+    <mergeCell ref="B88:E88"/>
+    <mergeCell ref="B83:K83"/>
+    <mergeCell ref="B84:E84"/>
+    <mergeCell ref="B85:E85"/>
+    <mergeCell ref="B86:E86"/>
+    <mergeCell ref="B92:E92"/>
+    <mergeCell ref="B38:M38"/>
+    <mergeCell ref="C101:G101"/>
+    <mergeCell ref="B71:E71"/>
+    <mergeCell ref="G71:H71"/>
+    <mergeCell ref="B79:E79"/>
+    <mergeCell ref="G80:H80"/>
+    <mergeCell ref="B80:E80"/>
+    <mergeCell ref="B69:H69"/>
+    <mergeCell ref="G76:H76"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="G70:H70"/>
+    <mergeCell ref="B87:E87"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="B44:H44"/>
+    <mergeCell ref="B72:H72"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="L99:M99"/>
+    <mergeCell ref="B97:K97"/>
+    <mergeCell ref="J62:M62"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="B81:E81"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="B70:E70"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="J5:K5"/>
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="B24:E24"/>
     <mergeCell ref="B7:D7"/>
@@ -2627,73 +2708,6 @@
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B1:M1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="L99:M99"/>
-    <mergeCell ref="B97:K97"/>
-    <mergeCell ref="J62:M62"/>
-    <mergeCell ref="G73:H73"/>
-    <mergeCell ref="B81:E81"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="B70:E70"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="B76:F76"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B38:M38"/>
-    <mergeCell ref="C101:G101"/>
-    <mergeCell ref="B71:E71"/>
-    <mergeCell ref="G71:H71"/>
-    <mergeCell ref="B79:E79"/>
-    <mergeCell ref="G80:H80"/>
-    <mergeCell ref="B80:E80"/>
-    <mergeCell ref="B69:H69"/>
-    <mergeCell ref="G76:H76"/>
-    <mergeCell ref="G65:H65"/>
-    <mergeCell ref="G70:H70"/>
-    <mergeCell ref="B87:E87"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="B43:H43"/>
-    <mergeCell ref="B44:H44"/>
-    <mergeCell ref="B72:H72"/>
-    <mergeCell ref="C104:F104"/>
-    <mergeCell ref="G79:H79"/>
-    <mergeCell ref="C102:G102"/>
-    <mergeCell ref="C100:G100"/>
-    <mergeCell ref="H102:I102"/>
-    <mergeCell ref="G81:H81"/>
-    <mergeCell ref="B88:E88"/>
-    <mergeCell ref="B83:K83"/>
-    <mergeCell ref="B84:E84"/>
-    <mergeCell ref="B85:E85"/>
-    <mergeCell ref="B86:E86"/>
-    <mergeCell ref="B92:E92"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="B46:H46"/>
-    <mergeCell ref="G74:H74"/>
-    <mergeCell ref="G78:H78"/>
-    <mergeCell ref="B77:E77"/>
-    <mergeCell ref="G77:H77"/>
-    <mergeCell ref="B74:E74"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>